<commit_message>
add update kanji file
</commit_message>
<xml_diff>
--- a/kanji.xlsx
+++ b/kanji.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21519"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21523"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{149FE650-DD2D-4342-BE77-13711CCB8E13}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0A73309-0229-4771-B7DD-84482009EF6A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28695" windowHeight="12525" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="28695" windowHeight="12525" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="1309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="1332">
   <si>
     <t>Chữ hán</t>
   </si>
@@ -3955,6 +3955,75 @@
   </si>
   <si>
     <t>thứ ~</t>
+  </si>
+  <si>
+    <t>急</t>
+  </si>
+  <si>
+    <t>Tốc</t>
+  </si>
+  <si>
+    <t>いそぎます</t>
+  </si>
+  <si>
+    <t>急ぎます</t>
+  </si>
+  <si>
+    <t>vội vàng</t>
+  </si>
+  <si>
+    <t>きゅうこう</t>
+  </si>
+  <si>
+    <t>急行</t>
+  </si>
+  <si>
+    <t>tàu tốc hành</t>
+  </si>
+  <si>
+    <t>とっきゅう</t>
+  </si>
+  <si>
+    <t>特急</t>
+  </si>
+  <si>
+    <t>tàu tốc hành đặc biệt</t>
+  </si>
+  <si>
+    <t>歌</t>
+  </si>
+  <si>
+    <t>Ca</t>
+  </si>
+  <si>
+    <t>うた</t>
+  </si>
+  <si>
+    <t>bài hát</t>
+  </si>
+  <si>
+    <t>うたいます</t>
+  </si>
+  <si>
+    <t>歌います</t>
+  </si>
+  <si>
+    <t>hát</t>
+  </si>
+  <si>
+    <t>終</t>
+  </si>
+  <si>
+    <t>Chung</t>
+  </si>
+  <si>
+    <t>おわります</t>
+  </si>
+  <si>
+    <t>終わります</t>
+  </si>
+  <si>
+    <t>kết thúc</t>
   </si>
 </sst>
 </file>
@@ -4346,10 +4415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H381"/>
+  <dimension ref="A1:H387"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="A369" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="E381" sqref="E381"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -4415,11 +4484,11 @@
       </c>
       <c r="G2" s="1">
         <f>COUNTA(A2:A100000)</f>
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H2" s="1">
         <f>COUNTA(C2:C10000)</f>
-        <v>380</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -9948,6 +10017,99 @@
       </c>
       <c r="F381" s="1">
         <v>19</v>
+      </c>
+    </row>
+    <row r="382" spans="1:6">
+      <c r="A382" s="1" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B382" s="1" t="s">
+        <v>1310</v>
+      </c>
+      <c r="C382" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="D382" s="1" t="s">
+        <v>1312</v>
+      </c>
+      <c r="E382" s="1" t="s">
+        <v>1313</v>
+      </c>
+      <c r="F382" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="383" spans="1:6">
+      <c r="C383" s="1" t="s">
+        <v>1314</v>
+      </c>
+      <c r="D383" s="1" t="s">
+        <v>1315</v>
+      </c>
+      <c r="E383" s="1" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="384" spans="1:6">
+      <c r="C384" s="1" t="s">
+        <v>1317</v>
+      </c>
+      <c r="D384" s="1" t="s">
+        <v>1318</v>
+      </c>
+      <c r="E384" s="1" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="385" spans="1:6">
+      <c r="A385" s="1" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B385" s="1" t="s">
+        <v>1321</v>
+      </c>
+      <c r="C385" s="1" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D385" s="1" t="s">
+        <v>1320</v>
+      </c>
+      <c r="E385" s="1" t="s">
+        <v>1323</v>
+      </c>
+      <c r="F385" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="386" spans="1:6">
+      <c r="C386" s="1" t="s">
+        <v>1324</v>
+      </c>
+      <c r="D386" s="1" t="s">
+        <v>1325</v>
+      </c>
+      <c r="E386" s="1" t="s">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="387" spans="1:6">
+      <c r="A387" s="1" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B387" s="1" t="s">
+        <v>1328</v>
+      </c>
+      <c r="C387" s="1" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D387" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="E387" s="1" t="s">
+        <v>1331</v>
+      </c>
+      <c r="F387" s="1">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -9962,7 +10124,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -9995,154 +10157,133 @@
     </row>
     <row r="2" spans="1:6" ht="18.75">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>1309</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>1310</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1312</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1313</v>
+      </c>
+      <c r="F2" s="1">
         <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18.75">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>1314</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>1315</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>1316</v>
+      </c>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="18.75">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>1317</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>1318</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>1319</v>
+      </c>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="18.75">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>1320</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>1321</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>1322</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>1320</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
+        <v>1323</v>
+      </c>
+      <c r="F5" s="1">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18.75">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>1324</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>1325</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>26</v>
-      </c>
+        <v>1326</v>
+      </c>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="18.75">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1328</v>
+      </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>1329</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>1330</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>1331</v>
+      </c>
+      <c r="F7" s="1">
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18.75">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="18.75">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="18.75">
-      <c r="A10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10">
-        <v>4</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="18.75">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update script and kanji file
</commit_message>
<xml_diff>
--- a/kanji.xlsx
+++ b/kanji.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21607"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34FDB1A1-A4D8-4DF2-9383-FF74C5D59A58}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{24025C9B-189C-44F3-8247-AB5CD7383B3D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="28695" windowHeight="12525" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="1412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1612" uniqueCount="1443">
   <si>
     <t>Chữ hán</t>
   </si>
@@ -4264,6 +4264,99 @@
   </si>
   <si>
     <t>bơi(v)</t>
+  </si>
+  <si>
+    <t>部</t>
+  </si>
+  <si>
+    <t>bộ</t>
+  </si>
+  <si>
+    <t>ぶちょう</t>
+  </si>
+  <si>
+    <t>部長</t>
+  </si>
+  <si>
+    <t>trưởng phòng</t>
+  </si>
+  <si>
+    <t>へや</t>
+  </si>
+  <si>
+    <t>部屋</t>
+  </si>
+  <si>
+    <t>căn phòng</t>
+  </si>
+  <si>
+    <t>ぜんぶ</t>
+  </si>
+  <si>
+    <t>全部</t>
+  </si>
+  <si>
+    <t>toàn bộ</t>
+  </si>
+  <si>
+    <t>khoa Y</t>
+  </si>
+  <si>
+    <t>屋</t>
+  </si>
+  <si>
+    <t>ốc</t>
+  </si>
+  <si>
+    <t>～や</t>
+  </si>
+  <si>
+    <t>～屋</t>
+  </si>
+  <si>
+    <t>hiệu ~</t>
+  </si>
+  <si>
+    <t>おくじょう</t>
+  </si>
+  <si>
+    <t>屋上</t>
+  </si>
+  <si>
+    <t>tầng thượng</t>
+  </si>
+  <si>
+    <t>室</t>
+  </si>
+  <si>
+    <t>thất</t>
+  </si>
+  <si>
+    <t>かいぎしつ</t>
+  </si>
+  <si>
+    <t>会議室</t>
+  </si>
+  <si>
+    <t>phòng họp</t>
+  </si>
+  <si>
+    <t>わしつ</t>
+  </si>
+  <si>
+    <t>和室</t>
+  </si>
+  <si>
+    <t>phòng kiểu nhật</t>
+  </si>
+  <si>
+    <t>ごうしつ</t>
+  </si>
+  <si>
+    <t>号室</t>
+  </si>
+  <si>
+    <t>số phòng</t>
   </si>
 </sst>
 </file>
@@ -4655,9 +4748,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H404"/>
+  <dimension ref="A1:H411"/>
   <sheetViews>
-    <sheetView topLeftCell="A247" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+    <sheetView topLeftCell="A398" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
       <selection activeCell="E263" sqref="E263"/>
     </sheetView>
   </sheetViews>
@@ -4724,11 +4817,11 @@
       </c>
       <c r="G2" s="1">
         <f>COUNTA(A2:A100005)</f>
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="H2" s="1">
         <f>COUNTA(C2:C10005)</f>
-        <v>403</v>
+        <v>410</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -10590,6 +10683,128 @@
         <v>1382</v>
       </c>
       <c r="F404" s="2"/>
+    </row>
+    <row r="405" spans="1:6">
+      <c r="A405" s="2" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B405" s="2" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C405" s="2" t="s">
+        <v>1385</v>
+      </c>
+      <c r="D405" s="2" t="s">
+        <v>1386</v>
+      </c>
+      <c r="E405" s="2" t="s">
+        <v>1387</v>
+      </c>
+      <c r="F405" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="406" spans="1:6">
+      <c r="A406" s="2"/>
+      <c r="B406" s="2"/>
+      <c r="C406" s="2" t="s">
+        <v>1388</v>
+      </c>
+      <c r="D406" s="2" t="s">
+        <v>1389</v>
+      </c>
+      <c r="E406" s="2" t="s">
+        <v>1390</v>
+      </c>
+      <c r="F406" s="2"/>
+    </row>
+    <row r="407" spans="1:6">
+      <c r="A407" s="2" t="s">
+        <v>1391</v>
+      </c>
+      <c r="B407" s="2" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C407" s="2" t="s">
+        <v>1393</v>
+      </c>
+      <c r="D407" s="2" t="s">
+        <v>1394</v>
+      </c>
+      <c r="E407" s="2" t="s">
+        <v>1395</v>
+      </c>
+      <c r="F407" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="408" spans="1:6">
+      <c r="A408" s="2" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B408" s="2" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C408" s="2" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D408" s="2" t="s">
+        <v>1399</v>
+      </c>
+      <c r="E408" s="2" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F408" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="409" spans="1:6">
+      <c r="A409" s="2"/>
+      <c r="B409" s="2"/>
+      <c r="C409" s="2" t="s">
+        <v>1401</v>
+      </c>
+      <c r="D409" s="2" t="s">
+        <v>1402</v>
+      </c>
+      <c r="E409" s="2" t="s">
+        <v>1403</v>
+      </c>
+      <c r="F409" s="2"/>
+    </row>
+    <row r="410" spans="1:6">
+      <c r="A410" s="2" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B410" s="2" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C410" s="2" t="s">
+        <v>1406</v>
+      </c>
+      <c r="D410" s="2" t="s">
+        <v>1407</v>
+      </c>
+      <c r="E410" s="2" t="s">
+        <v>1408</v>
+      </c>
+      <c r="F410" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="411" spans="1:6">
+      <c r="A411" s="2"/>
+      <c r="B411" s="2"/>
+      <c r="C411" s="2" t="s">
+        <v>1409</v>
+      </c>
+      <c r="D411" s="2" t="s">
+        <v>1410</v>
+      </c>
+      <c r="E411" s="2" t="s">
+        <v>1411</v>
+      </c>
+      <c r="F411" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E386" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
@@ -10600,10 +10815,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -10614,7 +10829,7 @@
     <col min="5" max="5" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75">
+    <row r="1" spans="1:18" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10634,135 +10849,519 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75">
+    <row r="2" spans="1:18" ht="18.75">
       <c r="A2" s="2" t="s">
-        <v>1383</v>
+        <v>1412</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1384</v>
+        <v>1413</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1385</v>
+        <v>1414</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>1386</v>
+        <v>1415</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>1387</v>
+        <v>1416</v>
       </c>
       <c r="F2" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="18.75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="18.75">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>1388</v>
+        <v>1417</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>1389</v>
+        <v>1418</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>1390</v>
+        <v>1419</v>
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="18.75">
-      <c r="A4" s="2" t="s">
-        <v>1391</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>1392</v>
-      </c>
+    <row r="4" spans="1:18" ht="18.75">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>1393</v>
+        <v>1420</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>1394</v>
+        <v>1421</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>1395</v>
-      </c>
-      <c r="F4" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="18.75">
-      <c r="A5" s="2" t="s">
-        <v>1396</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>1397</v>
-      </c>
+        <v>1422</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:18" ht="18.75">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>1398</v>
+        <v>173</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>1399</v>
+        <v>174</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>1400</v>
-      </c>
-      <c r="F5" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="18.75">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+        <v>1423</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:18" ht="18.75">
+      <c r="A6" s="2" t="s">
+        <v>1424</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1425</v>
+      </c>
       <c r="C6" s="2" t="s">
-        <v>1401</v>
+        <v>1417</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>1402</v>
+        <v>1418</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>1403</v>
-      </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" ht="18.75">
-      <c r="A7" s="2" t="s">
-        <v>1404</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>1405</v>
-      </c>
+        <v>1419</v>
+      </c>
+      <c r="F6" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="18.75">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>1406</v>
+        <v>1426</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>1407</v>
+        <v>1427</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>1408</v>
-      </c>
-      <c r="F7" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="18.75">
+        <v>1428</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:18" ht="18.75">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>1409</v>
+        <v>1429</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>1410</v>
+        <v>1430</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>1411</v>
+        <v>1431</v>
       </c>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" ht="18.75">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+    <row r="9" spans="1:18" ht="18.75">
+      <c r="A9" s="2" t="s">
+        <v>1432</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1433</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>887</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>888</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>889</v>
+      </c>
+      <c r="F9" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="18.75">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>1435</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>1436</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+    </row>
+    <row r="11" spans="1:18" ht="18.75">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>1437</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>1438</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>1439</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+    </row>
+    <row r="12" spans="1:18" ht="18.75">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>1388</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>1389</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>1390</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+    </row>
+    <row r="13" spans="1:18" ht="18.75">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>1441</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>1442</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+    </row>
+    <row r="14" spans="1:18" ht="18.75">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+    </row>
+    <row r="15" spans="1:18" ht="18.75">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+    </row>
+    <row r="16" spans="1:18" ht="18.75">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+    </row>
+    <row r="17" spans="1:18" ht="18.75">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+    </row>
+    <row r="18" spans="1:18" ht="18.75">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+    </row>
+    <row r="19" spans="1:18" ht="18.75">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+    </row>
+    <row r="20" spans="1:18" ht="18.75">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+    </row>
+    <row r="21" spans="1:18" ht="18.75">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+    </row>
+    <row r="22" spans="1:18" ht="18.75">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+    </row>
+    <row r="23" spans="1:18" ht="18.75">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+    </row>
+    <row r="24" spans="1:18" ht="18.75">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+    </row>
+    <row r="25" spans="1:18" ht="18.75">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+    </row>
+    <row r="26" spans="1:18" ht="18.75">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+    </row>
+    <row r="27" spans="1:18" ht="18.75">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update algorithm using level and day_down, add static chart
</commit_message>
<xml_diff>
--- a/kanji.xlsx
+++ b/kanji.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21705"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BFFA0313-C6EB-4F77-85F9-3A601F67151C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{80F1B2B3-79DF-4994-BC3B-46E684138EBE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28695" windowHeight="12525" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="28695" windowHeight="12525" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1725" uniqueCount="1542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1751" uniqueCount="1542">
   <si>
     <t>Chữ hán</t>
   </si>
@@ -5045,10 +5045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H448"/>
+  <dimension ref="A1:H454"/>
   <sheetViews>
-    <sheetView topLeftCell="A427" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="C443" sqref="C443"/>
+    <sheetView tabSelected="1" topLeftCell="A439" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="A449" sqref="A449"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -5114,11 +5114,11 @@
       </c>
       <c r="G2" s="1">
         <f>COUNTA(A2:A100005)</f>
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="H2" s="1">
         <f>COUNTA(C2:C10005)</f>
-        <v>447</v>
+        <v>453</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -11674,6 +11674,114 @@
       <c r="F448" s="2">
         <v>11</v>
       </c>
+    </row>
+    <row r="449" spans="1:6">
+      <c r="A449" s="2" t="s">
+        <v>1517</v>
+      </c>
+      <c r="B449" s="2" t="s">
+        <v>1518</v>
+      </c>
+      <c r="C449" s="2" t="s">
+        <v>1519</v>
+      </c>
+      <c r="D449" s="2" t="s">
+        <v>1520</v>
+      </c>
+      <c r="E449" s="2" t="s">
+        <v>1521</v>
+      </c>
+      <c r="F449" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="450" spans="1:6">
+      <c r="A450" s="2" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B450" s="2" t="s">
+        <v>1523</v>
+      </c>
+      <c r="C450" s="2" t="s">
+        <v>1524</v>
+      </c>
+      <c r="D450" s="2" t="s">
+        <v>1525</v>
+      </c>
+      <c r="E450" s="2" t="s">
+        <v>1526</v>
+      </c>
+      <c r="F450" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="451" spans="1:6">
+      <c r="A451" s="2"/>
+      <c r="B451" s="2"/>
+      <c r="C451" s="2" t="s">
+        <v>1527</v>
+      </c>
+      <c r="D451" s="2" t="s">
+        <v>1528</v>
+      </c>
+      <c r="E451" s="2" t="s">
+        <v>1529</v>
+      </c>
+      <c r="F451" s="2"/>
+    </row>
+    <row r="452" spans="1:6">
+      <c r="A452" s="2" t="s">
+        <v>1530</v>
+      </c>
+      <c r="B452" s="2" t="s">
+        <v>1308</v>
+      </c>
+      <c r="C452" s="2" t="s">
+        <v>1531</v>
+      </c>
+      <c r="D452" s="2" t="s">
+        <v>1532</v>
+      </c>
+      <c r="E452" s="2" t="s">
+        <v>1533</v>
+      </c>
+      <c r="F452" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="453" spans="1:6">
+      <c r="A453" s="2" t="s">
+        <v>1534</v>
+      </c>
+      <c r="B453" s="2" t="s">
+        <v>1535</v>
+      </c>
+      <c r="C453" s="2" t="s">
+        <v>1536</v>
+      </c>
+      <c r="D453" s="2" t="s">
+        <v>1537</v>
+      </c>
+      <c r="E453" s="2" t="s">
+        <v>1538</v>
+      </c>
+      <c r="F453" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="454" spans="1:6">
+      <c r="A454" s="2"/>
+      <c r="B454" s="2"/>
+      <c r="C454" s="2" t="s">
+        <v>1539</v>
+      </c>
+      <c r="D454" s="2" t="s">
+        <v>1540</v>
+      </c>
+      <c r="E454" s="2" t="s">
+        <v>1541</v>
+      </c>
+      <c r="F454" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E386" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
@@ -11686,8 +11794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+      <selection activeCell="A2" sqref="A2:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
update kanji and hours restudy
</commit_message>
<xml_diff>
--- a/kanji.xlsx
+++ b/kanji.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21705"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21715"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A6FDFDF-BF85-49DC-BFD5-A033BCB7FEEA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4501DB1C-A44E-4A1D-A557-37763C7A52D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28695" windowHeight="12525" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="28695" windowHeight="12525" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$364</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$367</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1885" uniqueCount="1693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1963" uniqueCount="1763">
   <si>
     <t>Chữ hán</t>
   </si>
@@ -3225,6 +3225,15 @@
     <t>cấm</t>
   </si>
   <si>
+    <t>たちいりきんし</t>
+  </si>
+  <si>
+    <t>立ち入り禁止</t>
+  </si>
+  <si>
+    <t>cấm vào</t>
+  </si>
+  <si>
     <t>雨</t>
   </si>
   <si>
@@ -3399,6 +3408,24 @@
     <t>đại sứ quán</t>
   </si>
   <si>
+    <t>しようきんし</t>
+  </si>
+  <si>
+    <t>使用禁止</t>
+  </si>
+  <si>
+    <t>cấm sử dụng</t>
+  </si>
+  <si>
+    <t>しようちゅう</t>
+  </si>
+  <si>
+    <t>使用中</t>
+  </si>
+  <si>
+    <t>đang sử dụng</t>
+  </si>
+  <si>
     <t>作</t>
   </si>
   <si>
@@ -5107,6 +5134,189 @@
   </si>
   <si>
     <t>chim</t>
+  </si>
+  <si>
+    <t>開</t>
+  </si>
+  <si>
+    <t>khai</t>
+  </si>
+  <si>
+    <t>あけます</t>
+  </si>
+  <si>
+    <t>開けます</t>
+  </si>
+  <si>
+    <t>mở(tha)</t>
+  </si>
+  <si>
+    <t>あきます</t>
+  </si>
+  <si>
+    <t>開きます</t>
+  </si>
+  <si>
+    <t>mở(tự)</t>
+  </si>
+  <si>
+    <t>ひらきます</t>
+  </si>
+  <si>
+    <t>mở(công ty)</t>
+  </si>
+  <si>
+    <t>かいはつします</t>
+  </si>
+  <si>
+    <t>開発します</t>
+  </si>
+  <si>
+    <t>phát triển</t>
+  </si>
+  <si>
+    <t>閉</t>
+  </si>
+  <si>
+    <t>bế</t>
+  </si>
+  <si>
+    <t>しめます</t>
+  </si>
+  <si>
+    <t>閉めます</t>
+  </si>
+  <si>
+    <t>đóng(tha)</t>
+  </si>
+  <si>
+    <t>しまります</t>
+  </si>
+  <si>
+    <t>閉まります</t>
+  </si>
+  <si>
+    <t>đóng(tự)</t>
+  </si>
+  <si>
+    <t>とじます</t>
+  </si>
+  <si>
+    <t>閉じます</t>
+  </si>
+  <si>
+    <t>nhắm</t>
+  </si>
+  <si>
+    <t>持</t>
+  </si>
+  <si>
+    <t>trì</t>
+  </si>
+  <si>
+    <t>もちます</t>
+  </si>
+  <si>
+    <t>持ちます</t>
+  </si>
+  <si>
+    <t>lấy</t>
+  </si>
+  <si>
+    <t>もっていきます</t>
+  </si>
+  <si>
+    <t>持っていきます</t>
+  </si>
+  <si>
+    <t>mang đi</t>
+  </si>
+  <si>
+    <t>もってきます</t>
+  </si>
+  <si>
+    <t>持ってきます</t>
+  </si>
+  <si>
+    <t>mang đến</t>
+  </si>
+  <si>
+    <t>きもち</t>
+  </si>
+  <si>
+    <t>気持ち</t>
+  </si>
+  <si>
+    <t>cảm xúc</t>
+  </si>
+  <si>
+    <t>住</t>
+  </si>
+  <si>
+    <t>trụ(trú)</t>
+  </si>
+  <si>
+    <t>すみます</t>
+  </si>
+  <si>
+    <t>住みます</t>
+  </si>
+  <si>
+    <t>乗</t>
+  </si>
+  <si>
+    <t>thừa</t>
+  </si>
+  <si>
+    <t>nơi lên xe</t>
+  </si>
+  <si>
+    <t>のります</t>
+  </si>
+  <si>
+    <t>乗ります</t>
+  </si>
+  <si>
+    <t>lên xe</t>
+  </si>
+  <si>
+    <t>のりかえます</t>
+  </si>
+  <si>
+    <t>乗り換えます</t>
+  </si>
+  <si>
+    <t>chuyển xe</t>
+  </si>
+  <si>
+    <t>降</t>
+  </si>
+  <si>
+    <t>hàng(giáng)</t>
+  </si>
+  <si>
+    <t>ふります</t>
+  </si>
+  <si>
+    <t>降ります</t>
+  </si>
+  <si>
+    <t>rơi</t>
+  </si>
+  <si>
+    <t>おります</t>
+  </si>
+  <si>
+    <t>xuống xe</t>
+  </si>
+  <si>
+    <t>おろします</t>
+  </si>
+  <si>
+    <t>降ろします</t>
+  </si>
+  <si>
+    <t>cho xuống xe</t>
   </si>
 </sst>
 </file>
@@ -5498,10 +5708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H488"/>
+  <dimension ref="A1:H505"/>
   <sheetViews>
-    <sheetView topLeftCell="A486" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="A489" sqref="A489:F502"/>
+    <sheetView topLeftCell="A465" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="D472" sqref="D472"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -5566,12 +5776,12 @@
         <v>4</v>
       </c>
       <c r="G2" s="1">
-        <f>COUNTA(A2:A100039)</f>
-        <v>176</v>
+        <f>COUNTA(A2:A100042)</f>
+        <v>184</v>
       </c>
       <c r="H2" s="1">
-        <f>COUNTA(C2:C10039)</f>
-        <v>487</v>
+        <f>COUNTA(C2:C10042)</f>
+        <v>504</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -10012,34 +10222,34 @@
       </c>
     </row>
     <row r="315" spans="1:6">
-      <c r="A315" s="1" t="s">
+      <c r="C315" s="1" t="s">
         <v>1065</v>
       </c>
-      <c r="B315" s="1" t="s">
+      <c r="D315" s="1" t="s">
         <v>1066</v>
       </c>
-      <c r="C315" s="1" t="s">
+      <c r="E315" s="1" t="s">
         <v>1067</v>
       </c>
-      <c r="D315" s="1" t="s">
-        <v>1065</v>
-      </c>
-      <c r="E315" s="1" t="s">
+    </row>
+    <row r="316" spans="1:6">
+      <c r="A316" s="1" t="s">
         <v>1068</v>
       </c>
-      <c r="F315" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="316" spans="1:6">
+      <c r="B316" s="1" t="s">
+        <v>1069</v>
+      </c>
       <c r="C316" s="1" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="D316" s="1" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="E316" s="1" t="s">
         <v>1071</v>
+      </c>
+      <c r="F316" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="317" spans="1:6">
@@ -10054,26 +10264,23 @@
       </c>
     </row>
     <row r="318" spans="1:6">
-      <c r="A318" s="1" t="s">
+      <c r="C318" s="1" t="s">
         <v>1075</v>
       </c>
-      <c r="B318" s="1" t="s">
+      <c r="D318" s="1" t="s">
         <v>1076</v>
       </c>
-      <c r="C318" s="1" t="s">
+      <c r="E318" s="1" t="s">
         <v>1077</v>
       </c>
-      <c r="D318" s="1" t="s">
+    </row>
+    <row r="319" spans="1:6">
+      <c r="A319" s="1" t="s">
         <v>1078</v>
       </c>
-      <c r="E318" s="1" t="s">
+      <c r="B319" s="1" t="s">
         <v>1079</v>
       </c>
-      <c r="F318" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="319" spans="1:6">
       <c r="C319" s="1" t="s">
         <v>1080</v>
       </c>
@@ -10082,6 +10289,9 @@
       </c>
       <c r="E319" s="1" t="s">
         <v>1082</v>
+      </c>
+      <c r="F319" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="320" spans="1:6">
@@ -10107,26 +10317,23 @@
       </c>
     </row>
     <row r="322" spans="1:6">
-      <c r="A322" s="1" t="s">
+      <c r="C322" s="1" t="s">
         <v>1089</v>
       </c>
-      <c r="B322" s="1" t="s">
+      <c r="D322" s="1" t="s">
         <v>1090</v>
       </c>
-      <c r="C322" s="1" t="s">
+      <c r="E322" s="1" t="s">
         <v>1091</v>
       </c>
-      <c r="D322" s="1" t="s">
+    </row>
+    <row r="323" spans="1:6">
+      <c r="A323" s="1" t="s">
         <v>1092</v>
       </c>
-      <c r="E322" s="1" t="s">
+      <c r="B323" s="1" t="s">
         <v>1093</v>
       </c>
-      <c r="F322" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="323" spans="1:6">
       <c r="C323" s="1" t="s">
         <v>1094</v>
       </c>
@@ -10135,6 +10342,9 @@
       </c>
       <c r="E323" s="1" t="s">
         <v>1096</v>
+      </c>
+      <c r="F323" s="1">
+        <v>5</v>
       </c>
     </row>
     <row r="324" spans="1:6">
@@ -10160,26 +10370,23 @@
       </c>
     </row>
     <row r="326" spans="1:6">
-      <c r="A326" s="1" t="s">
+      <c r="C326" s="1" t="s">
         <v>1103</v>
       </c>
-      <c r="B326" s="1" t="s">
+      <c r="D326" s="1" t="s">
         <v>1104</v>
       </c>
-      <c r="C326" s="1" t="s">
+      <c r="E326" s="1" t="s">
         <v>1105</v>
       </c>
-      <c r="D326" s="1" t="s">
+    </row>
+    <row r="327" spans="1:6">
+      <c r="A327" s="1" t="s">
         <v>1106</v>
       </c>
-      <c r="E326" s="1" t="s">
+      <c r="B327" s="1" t="s">
         <v>1107</v>
       </c>
-      <c r="F326" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="327" spans="1:6">
       <c r="C327" s="1" t="s">
         <v>1108</v>
       </c>
@@ -10189,50 +10396,50 @@
       <c r="E327" s="1" t="s">
         <v>1110</v>
       </c>
+      <c r="F327" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="328" spans="1:6">
       <c r="C328" s="1" t="s">
-        <v>496</v>
+        <v>1111</v>
       </c>
       <c r="D328" s="1" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="E328" s="1" t="s">
-        <v>498</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="329" spans="1:6">
       <c r="C329" s="1" t="s">
-        <v>1112</v>
+        <v>496</v>
       </c>
       <c r="D329" s="1" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="E329" s="1" t="s">
-        <v>1114</v>
+        <v>498</v>
       </c>
     </row>
     <row r="330" spans="1:6">
-      <c r="A330" s="1" t="s">
+      <c r="C330" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="B330" s="1" t="s">
+      <c r="D330" s="1" t="s">
         <v>1116</v>
       </c>
-      <c r="C330" s="1" t="s">
+      <c r="E330" s="1" t="s">
         <v>1117</v>
       </c>
-      <c r="D330" s="1" t="s">
+    </row>
+    <row r="331" spans="1:6">
+      <c r="A331" s="1" t="s">
         <v>1118</v>
       </c>
-      <c r="E330" s="1" t="s">
+      <c r="B331" s="1" t="s">
         <v>1119</v>
       </c>
-      <c r="F330" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="331" spans="1:6">
       <c r="C331" s="1" t="s">
         <v>1120</v>
       </c>
@@ -10242,121 +10449,121 @@
       <c r="E331" s="1" t="s">
         <v>1122</v>
       </c>
+      <c r="F331" s="1">
+        <v>8</v>
+      </c>
     </row>
     <row r="332" spans="1:6">
-      <c r="A332" s="1" t="s">
+      <c r="C332" s="1" t="s">
         <v>1123</v>
       </c>
-      <c r="B332" s="1" t="s">
+      <c r="D332" s="1" t="s">
         <v>1124</v>
       </c>
-      <c r="C332" s="1" t="s">
+      <c r="E332" s="1" t="s">
         <v>1125</v>
-      </c>
-      <c r="D332" s="1" t="s">
-        <v>1126</v>
-      </c>
-      <c r="E332" s="1" t="s">
-        <v>1127</v>
-      </c>
-      <c r="F332" s="1">
-        <v>7</v>
       </c>
     </row>
     <row r="333" spans="1:6">
       <c r="C333" s="1" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D333" s="1" t="s">
+        <v>1127</v>
+      </c>
+      <c r="E333" s="1" t="s">
         <v>1128</v>
       </c>
-      <c r="D333" s="1" t="s">
+    </row>
+    <row r="334" spans="1:6">
+      <c r="C334" s="1" t="s">
         <v>1129</v>
       </c>
-      <c r="E333" s="1" t="s">
+      <c r="D334" s="1" t="s">
         <v>1130</v>
       </c>
-    </row>
-    <row r="334" spans="1:6">
-      <c r="A334" s="1" t="s">
+      <c r="E334" s="1" t="s">
         <v>1131</v>
-      </c>
-      <c r="B334" s="1" t="s">
-        <v>1132</v>
-      </c>
-      <c r="C334" s="1" t="s">
-        <v>1133</v>
-      </c>
-      <c r="D334" s="1" t="s">
-        <v>1134</v>
-      </c>
-      <c r="E334" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="F334" s="1">
-        <v>9</v>
       </c>
     </row>
     <row r="335" spans="1:6">
       <c r="A335" s="1" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B335" s="1" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C335" s="1" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D335" s="1" t="s">
         <v>1135</v>
       </c>
-      <c r="B335" s="1" t="s">
+      <c r="E335" s="1" t="s">
         <v>1136</v>
       </c>
-      <c r="C335" s="1" t="s">
+      <c r="F335" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="336" spans="1:6">
+      <c r="C336" s="1" t="s">
         <v>1137</v>
       </c>
-      <c r="D335" s="1" t="s">
+      <c r="D336" s="1" t="s">
         <v>1138</v>
       </c>
-      <c r="E335" s="1" t="s">
+      <c r="E336" s="1" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6">
+      <c r="A337" s="1" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B337" s="1" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C337" s="1" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D337" s="1" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E337" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="F337" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="338" spans="1:6">
+      <c r="A338" s="1" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B338" s="1" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C338" s="1" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D338" s="1" t="s">
+        <v>1147</v>
+      </c>
+      <c r="E338" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="F335" s="1">
+      <c r="F338" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="336" spans="1:6">
-      <c r="A336" s="1" t="s">
-        <v>1139</v>
-      </c>
-      <c r="B336" s="1" t="s">
-        <v>1140</v>
-      </c>
-      <c r="C336" s="1" t="s">
-        <v>1141</v>
-      </c>
-      <c r="D336" s="1" t="s">
-        <v>1142</v>
-      </c>
-      <c r="E336" s="1" t="s">
-        <v>1143</v>
-      </c>
-      <c r="F336" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="337" spans="1:6">
-      <c r="C337" s="1" t="s">
-        <v>1144</v>
-      </c>
-      <c r="D337" s="1" t="s">
-        <v>1145</v>
-      </c>
-      <c r="E337" s="1" t="s">
-        <v>1146</v>
-      </c>
-    </row>
-    <row r="338" spans="1:6">
-      <c r="C338" s="1" t="s">
-        <v>1147</v>
-      </c>
-      <c r="D338" s="1" t="s">
+    <row r="339" spans="1:6">
+      <c r="A339" s="1" t="s">
         <v>1148</v>
       </c>
-      <c r="E338" s="1" t="s">
+      <c r="B339" s="1" t="s">
         <v>1149</v>
       </c>
-    </row>
-    <row r="339" spans="1:6">
       <c r="C339" s="1" t="s">
         <v>1150</v>
       </c>
@@ -10366,227 +10573,227 @@
       <c r="E339" s="1" t="s">
         <v>1152</v>
       </c>
+      <c r="F339" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="340" spans="1:6">
-      <c r="A340" s="1" t="s">
+      <c r="C340" s="1" t="s">
         <v>1153</v>
       </c>
-      <c r="B340" s="1" t="s">
+      <c r="D340" s="1" t="s">
         <v>1154</v>
       </c>
-      <c r="C340" s="1" t="s">
+      <c r="E340" s="1" t="s">
         <v>1155</v>
       </c>
-      <c r="D340" s="1" t="s">
+    </row>
+    <row r="341" spans="1:6">
+      <c r="C341" s="1" t="s">
         <v>1156</v>
       </c>
-      <c r="E340" s="1" t="s">
+      <c r="D341" s="1" t="s">
         <v>1157</v>
       </c>
-      <c r="F340" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="341" spans="1:6">
-      <c r="A341" s="1" t="s">
+      <c r="E341" s="1" t="s">
         <v>1158</v>
-      </c>
-      <c r="B341" s="1" t="s">
-        <v>1159</v>
-      </c>
-      <c r="C341" s="1" t="s">
-        <v>1160</v>
-      </c>
-      <c r="D341" s="1" t="s">
-        <v>1161</v>
-      </c>
-      <c r="E341" s="1" t="s">
-        <v>1162</v>
-      </c>
-      <c r="F341" s="1">
-        <v>4</v>
       </c>
     </row>
     <row r="342" spans="1:6">
       <c r="C342" s="1" t="s">
+        <v>1159</v>
+      </c>
+      <c r="D342" s="1" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E342" s="1" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="343" spans="1:6">
+      <c r="A343" s="1" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B343" s="1" t="s">
         <v>1163</v>
       </c>
-      <c r="D342" s="1" t="s">
+      <c r="C343" s="1" t="s">
         <v>1164</v>
       </c>
-      <c r="E342" s="1" t="s">
+      <c r="D343" s="1" t="s">
         <v>1165</v>
       </c>
-    </row>
-    <row r="343" spans="1:6">
-      <c r="C343" s="1" t="s">
+      <c r="E343" s="1" t="s">
         <v>1166</v>
       </c>
-      <c r="D343" s="1" t="s">
-        <v>1167</v>
-      </c>
-      <c r="E343" s="1" t="s">
-        <v>1168</v>
+      <c r="F343" s="1">
+        <v>6</v>
       </c>
     </row>
     <row r="344" spans="1:6">
       <c r="A344" s="1" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B344" s="1" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C344" s="1" t="s">
         <v>1169</v>
       </c>
-      <c r="B344" s="1" t="s">
+      <c r="D344" s="1" t="s">
         <v>1170</v>
       </c>
-      <c r="C344" s="1" t="s">
+      <c r="E344" s="1" t="s">
         <v>1171</v>
       </c>
-      <c r="D344" s="1" t="s">
-        <v>1172</v>
-      </c>
-      <c r="E344" s="1" t="s">
-        <v>1173</v>
-      </c>
       <c r="F344" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="345" spans="1:6">
       <c r="C345" s="1" t="s">
+        <v>1172</v>
+      </c>
+      <c r="D345" s="1" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E345" s="1" t="s">
         <v>1174</v>
-      </c>
-      <c r="D345" s="1" t="s">
-        <v>1175</v>
-      </c>
-      <c r="E345" s="1" t="s">
-        <v>1176</v>
       </c>
     </row>
     <row r="346" spans="1:6">
       <c r="C346" s="1" t="s">
-        <v>178</v>
+        <v>1175</v>
       </c>
       <c r="D346" s="1" t="s">
-        <v>179</v>
+        <v>1176</v>
       </c>
       <c r="E346" s="1" t="s">
-        <v>180</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="347" spans="1:6">
+      <c r="A347" s="1" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B347" s="1" t="s">
+        <v>1179</v>
+      </c>
       <c r="C347" s="1" t="s">
-        <v>1177</v>
+        <v>1180</v>
       </c>
       <c r="D347" s="1" t="s">
-        <v>1178</v>
+        <v>1181</v>
       </c>
       <c r="E347" s="1" t="s">
-        <v>1179</v>
+        <v>1182</v>
+      </c>
+      <c r="F347" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="348" spans="1:6">
-      <c r="A348" s="1" t="s">
-        <v>1180</v>
-      </c>
-      <c r="B348" s="1" t="s">
-        <v>1181</v>
-      </c>
       <c r="C348" s="1" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="D348" s="1" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="E348" s="1" t="s">
-        <v>1184</v>
-      </c>
-      <c r="F348" s="1">
-        <v>12</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="349" spans="1:6">
       <c r="C349" s="1" t="s">
-        <v>1185</v>
+        <v>178</v>
       </c>
       <c r="D349" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E349" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="350" spans="1:6">
+      <c r="C350" s="1" t="s">
         <v>1186</v>
       </c>
-      <c r="E349" s="1" t="s">
+      <c r="D350" s="1" t="s">
         <v>1187</v>
       </c>
-    </row>
-    <row r="350" spans="1:6">
-      <c r="A350" s="1" t="s">
+      <c r="E350" s="1" t="s">
         <v>1188</v>
       </c>
-      <c r="B350" s="1" t="s">
+    </row>
+    <row r="351" spans="1:6">
+      <c r="A351" s="1" t="s">
         <v>1189</v>
       </c>
-      <c r="C350" s="1" t="s">
+      <c r="B351" s="1" t="s">
         <v>1190</v>
       </c>
-      <c r="D350" s="1" t="s">
+      <c r="C351" s="1" t="s">
         <v>1191</v>
       </c>
-      <c r="E350" s="1" t="s">
+      <c r="D351" s="1" t="s">
         <v>1192</v>
       </c>
-      <c r="F350" s="1">
+      <c r="E351" s="1" t="s">
+        <v>1193</v>
+      </c>
+      <c r="F351" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="352" spans="1:6">
+      <c r="C352" s="1" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D352" s="1" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E352" s="1" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="353" spans="1:6">
+      <c r="A353" s="1" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B353" s="1" t="s">
+        <v>1198</v>
+      </c>
+      <c r="C353" s="1" t="s">
+        <v>1199</v>
+      </c>
+      <c r="D353" s="1" t="s">
+        <v>1200</v>
+      </c>
+      <c r="E353" s="1" t="s">
+        <v>1201</v>
+      </c>
+      <c r="F353" s="1">
         <v>11</v>
-      </c>
-    </row>
-    <row r="351" spans="1:6">
-      <c r="C351" s="1" t="s">
-        <v>1193</v>
-      </c>
-      <c r="D351" s="1" t="s">
-        <v>1194</v>
-      </c>
-      <c r="E351" s="1" t="s">
-        <v>1195</v>
-      </c>
-    </row>
-    <row r="352" spans="1:6">
-      <c r="A352" s="1" t="s">
-        <v>1196</v>
-      </c>
-      <c r="B352" s="1" t="s">
-        <v>1197</v>
-      </c>
-      <c r="C352" s="1" t="s">
-        <v>1198</v>
-      </c>
-      <c r="D352" s="1" t="s">
-        <v>1199</v>
-      </c>
-      <c r="E352" s="1" t="s">
-        <v>1200</v>
-      </c>
-      <c r="F352" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="353" spans="1:6">
-      <c r="C353" s="1" t="s">
-        <v>1201</v>
-      </c>
-      <c r="D353" s="1" t="s">
-        <v>1202</v>
-      </c>
-      <c r="E353" s="1" t="s">
-        <v>1203</v>
       </c>
     </row>
     <row r="354" spans="1:6">
       <c r="C354" s="1" t="s">
+        <v>1202</v>
+      </c>
+      <c r="D354" s="1" t="s">
+        <v>1203</v>
+      </c>
+      <c r="E354" s="1" t="s">
         <v>1204</v>
       </c>
-      <c r="D354" s="1" t="s">
+    </row>
+    <row r="355" spans="1:6">
+      <c r="A355" s="1" t="s">
         <v>1205</v>
       </c>
-      <c r="E354" s="1" t="s">
+      <c r="B355" s="1" t="s">
         <v>1206</v>
       </c>
-    </row>
-    <row r="355" spans="1:6">
       <c r="C355" s="1" t="s">
         <v>1207</v>
       </c>
@@ -10595,6 +10802,9 @@
       </c>
       <c r="E355" s="1" t="s">
         <v>1209</v>
+      </c>
+      <c r="F355" s="1">
+        <v>9</v>
       </c>
     </row>
     <row r="356" spans="1:6">
@@ -10605,52 +10815,49 @@
         <v>1211</v>
       </c>
       <c r="E356" s="1" t="s">
-        <v>936</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="357" spans="1:6">
-      <c r="A357" s="1" t="s">
-        <v>1212</v>
-      </c>
-      <c r="B357" s="1" t="s">
+      <c r="C357" s="1" t="s">
         <v>1213</v>
       </c>
-      <c r="C357" s="1" t="s">
+      <c r="D357" s="1" t="s">
         <v>1214</v>
       </c>
-      <c r="D357" s="1" t="s">
+      <c r="E357" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="E357" s="1" t="s">
-        <v>1216</v>
-      </c>
-      <c r="F357" s="1">
-        <v>12</v>
       </c>
     </row>
     <row r="358" spans="1:6">
       <c r="C358" s="1" t="s">
+        <v>1216</v>
+      </c>
+      <c r="D358" s="1" t="s">
         <v>1217</v>
       </c>
-      <c r="D358" s="1" t="s">
+      <c r="E358" s="1" t="s">
         <v>1218</v>
-      </c>
-      <c r="E358" s="1" t="s">
-        <v>1219</v>
       </c>
     </row>
     <row r="359" spans="1:6">
       <c r="C359" s="1" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D359" s="1" t="s">
         <v>1220</v>
       </c>
-      <c r="D359" s="1" t="s">
+      <c r="E359" s="1" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6">
+      <c r="A360" s="1" t="s">
         <v>1221</v>
       </c>
-      <c r="E359" s="1" t="s">
+      <c r="B360" s="1" t="s">
         <v>1222</v>
       </c>
-    </row>
-    <row r="360" spans="1:6">
       <c r="C360" s="1" t="s">
         <v>1223</v>
       </c>
@@ -10660,50 +10867,50 @@
       <c r="E360" s="1" t="s">
         <v>1225</v>
       </c>
+      <c r="F360" s="1">
+        <v>12</v>
+      </c>
     </row>
     <row r="361" spans="1:6">
-      <c r="A361" s="1" t="s">
+      <c r="C361" s="1" t="s">
         <v>1226</v>
       </c>
-      <c r="B361" s="1" t="s">
+      <c r="D361" s="1" t="s">
         <v>1227</v>
       </c>
-      <c r="C361" s="1" t="s">
+      <c r="E361" s="1" t="s">
         <v>1228</v>
-      </c>
-      <c r="D361" s="1" t="s">
-        <v>1229</v>
-      </c>
-      <c r="E361" s="1" t="s">
-        <v>1230</v>
-      </c>
-      <c r="F361" s="1">
-        <v>6</v>
       </c>
     </row>
     <row r="362" spans="1:6">
       <c r="C362" s="1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D362" s="1" t="s">
+        <v>1230</v>
+      </c>
+      <c r="E362" s="1" t="s">
         <v>1231</v>
-      </c>
-      <c r="D362" s="1" t="s">
-        <v>1232</v>
-      </c>
-      <c r="E362" s="1" t="s">
-        <v>1233</v>
       </c>
     </row>
     <row r="363" spans="1:6">
       <c r="C363" s="1" t="s">
+        <v>1232</v>
+      </c>
+      <c r="D363" s="1" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E363" s="1" t="s">
         <v>1234</v>
       </c>
-      <c r="D363" s="1" t="s">
+    </row>
+    <row r="364" spans="1:6">
+      <c r="A364" s="1" t="s">
         <v>1235</v>
       </c>
-      <c r="E363" s="1" t="s">
+      <c r="B364" s="1" t="s">
         <v>1236</v>
       </c>
-    </row>
-    <row r="364" spans="1:6">
       <c r="C364" s="1" t="s">
         <v>1237</v>
       </c>
@@ -10713,171 +10920,165 @@
       <c r="E364" s="1" t="s">
         <v>1239</v>
       </c>
+      <c r="F364" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="365" spans="1:6">
-      <c r="A365" s="1" t="s">
+      <c r="C365" s="1" t="s">
         <v>1240</v>
       </c>
-      <c r="B365" s="1" t="s">
+      <c r="D365" s="1" t="s">
         <v>1241</v>
       </c>
-      <c r="C365" s="1" t="s">
+      <c r="E365" s="1" t="s">
         <v>1242</v>
       </c>
-      <c r="D365" s="1" t="s">
+    </row>
+    <row r="366" spans="1:6">
+      <c r="C366" s="1" t="s">
         <v>1243</v>
       </c>
-      <c r="E365" s="1" t="s">
+      <c r="D366" s="1" t="s">
         <v>1244</v>
       </c>
-      <c r="F365" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="366" spans="1:6">
-      <c r="A366" s="1" t="s">
+      <c r="E366" s="1" t="s">
         <v>1245</v>
-      </c>
-      <c r="B366" s="1" t="s">
-        <v>1246</v>
-      </c>
-      <c r="C366" s="1" t="s">
-        <v>1247</v>
-      </c>
-      <c r="D366" s="1" t="s">
-        <v>1248</v>
-      </c>
-      <c r="E366" s="1" t="s">
-        <v>1249</v>
-      </c>
-      <c r="F366" s="1">
-        <v>7</v>
       </c>
     </row>
     <row r="367" spans="1:6">
       <c r="C367" s="1" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D367" s="1" t="s">
+        <v>1247</v>
+      </c>
+      <c r="E367" s="1" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="368" spans="1:6">
+      <c r="A368" s="1" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B368" s="1" t="s">
         <v>1250</v>
       </c>
-      <c r="D367" s="1" t="s">
+      <c r="C368" s="1" t="s">
         <v>1251</v>
       </c>
-      <c r="E367" s="1" t="s">
+      <c r="D368" s="1" t="s">
         <v>1252</v>
       </c>
-    </row>
-    <row r="368" spans="1:6">
-      <c r="C368" s="1" t="s">
+      <c r="E368" s="1" t="s">
         <v>1253</v>
       </c>
-      <c r="D368" s="1" t="s">
-        <v>1254</v>
-      </c>
-      <c r="E368" s="1" t="s">
-        <v>1255</v>
+      <c r="F368" s="1">
+        <v>9</v>
       </c>
     </row>
     <row r="369" spans="1:6">
       <c r="A369" s="1" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B369" s="1" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C369" s="1" t="s">
         <v>1256</v>
       </c>
-      <c r="B369" s="1" t="s">
+      <c r="D369" s="1" t="s">
         <v>1257</v>
       </c>
-      <c r="C369" s="1" t="s">
+      <c r="E369" s="1" t="s">
         <v>1258</v>
       </c>
-      <c r="D369" s="1" t="s">
-        <v>1256</v>
-      </c>
-      <c r="E369" s="1" t="s">
+      <c r="F369" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="370" spans="1:6">
+      <c r="C370" s="1" t="s">
         <v>1259</v>
       </c>
-      <c r="F369" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="370" spans="1:6">
-      <c r="A370" s="1" t="s">
+      <c r="D370" s="1" t="s">
         <v>1260</v>
       </c>
-      <c r="B370" s="1" t="s">
+      <c r="E370" s="1" t="s">
         <v>1261</v>
-      </c>
-      <c r="C370" s="1" t="s">
-        <v>1262</v>
-      </c>
-      <c r="D370" s="1" t="s">
-        <v>1263</v>
-      </c>
-      <c r="E370" s="1" t="s">
-        <v>1264</v>
-      </c>
-      <c r="F370" s="1">
-        <v>6</v>
       </c>
     </row>
     <row r="371" spans="1:6">
       <c r="C371" s="1" t="s">
+        <v>1262</v>
+      </c>
+      <c r="D371" s="1" t="s">
+        <v>1263</v>
+      </c>
+      <c r="E371" s="1" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="372" spans="1:6">
+      <c r="A372" s="1" t="s">
         <v>1265</v>
       </c>
-      <c r="D371" s="1" t="s">
+      <c r="B372" s="1" t="s">
         <v>1266</v>
       </c>
-      <c r="E371" s="1" t="s">
+      <c r="C372" s="1" t="s">
         <v>1267</v>
       </c>
-    </row>
-    <row r="372" spans="1:6">
-      <c r="C372" s="1" t="s">
-        <v>465</v>
-      </c>
       <c r="D372" s="1" t="s">
-        <v>466</v>
+        <v>1265</v>
       </c>
       <c r="E372" s="1" t="s">
-        <v>467</v>
+        <v>1268</v>
+      </c>
+      <c r="F372" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="373" spans="1:6">
+      <c r="A373" s="1" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B373" s="1" t="s">
+        <v>1270</v>
+      </c>
       <c r="C373" s="1" t="s">
-        <v>1268</v>
+        <v>1271</v>
       </c>
       <c r="D373" s="1" t="s">
-        <v>1269</v>
+        <v>1272</v>
       </c>
       <c r="E373" s="1" t="s">
-        <v>1270</v>
+        <v>1273</v>
+      </c>
+      <c r="F373" s="1">
+        <v>6</v>
       </c>
     </row>
     <row r="374" spans="1:6">
       <c r="C374" s="1" t="s">
-        <v>1271</v>
+        <v>1274</v>
       </c>
       <c r="D374" s="1" t="s">
-        <v>1272</v>
+        <v>1275</v>
       </c>
       <c r="E374" s="1" t="s">
-        <v>1273</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="375" spans="1:6">
-      <c r="A375" s="1" t="s">
-        <v>1274</v>
-      </c>
-      <c r="B375" s="1" t="s">
-        <v>1275</v>
-      </c>
       <c r="C375" s="1" t="s">
-        <v>931</v>
+        <v>465</v>
       </c>
       <c r="D375" s="1" t="s">
-        <v>932</v>
+        <v>466</v>
       </c>
       <c r="E375" s="1" t="s">
-        <v>1276</v>
-      </c>
-      <c r="F375" s="1">
-        <v>16</v>
+        <v>467</v>
       </c>
     </row>
     <row r="376" spans="1:6">
@@ -10885,167 +11086,167 @@
         <v>1277</v>
       </c>
       <c r="D376" s="1" t="s">
-        <v>1274</v>
+        <v>1278</v>
       </c>
       <c r="E376" s="1" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="377" spans="1:6">
       <c r="C377" s="1" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="D377" s="1" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="E377" s="1" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="378" spans="1:6">
+      <c r="A378" s="1" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B378" s="1" t="s">
+        <v>1284</v>
+      </c>
       <c r="C378" s="1" t="s">
-        <v>1282</v>
+        <v>931</v>
       </c>
       <c r="D378" s="1" t="s">
-        <v>1283</v>
+        <v>932</v>
       </c>
       <c r="E378" s="1" t="s">
-        <v>1284</v>
+        <v>1285</v>
+      </c>
+      <c r="F378" s="1">
+        <v>16</v>
       </c>
     </row>
     <row r="379" spans="1:6">
       <c r="C379" s="1" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="D379" s="1" t="s">
-        <v>1286</v>
+        <v>1283</v>
       </c>
       <c r="E379" s="1" t="s">
         <v>1287</v>
       </c>
     </row>
     <row r="380" spans="1:6">
-      <c r="A380" s="1" t="s">
+      <c r="C380" s="1" t="s">
         <v>1288</v>
       </c>
-      <c r="B380" s="1" t="s">
-        <v>747</v>
-      </c>
-      <c r="C380" s="1" t="s">
+      <c r="D380" s="1" t="s">
         <v>1289</v>
       </c>
-      <c r="D380" s="1" t="s">
+      <c r="E380" s="1" t="s">
         <v>1290</v>
-      </c>
-      <c r="E380" s="1" t="s">
-        <v>1291</v>
-      </c>
-      <c r="F380" s="1">
-        <v>6</v>
       </c>
     </row>
     <row r="381" spans="1:6">
       <c r="C381" s="1" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D381" s="1" t="s">
         <v>1292</v>
       </c>
-      <c r="D381" s="1" t="s">
+      <c r="E381" s="1" t="s">
         <v>1293</v>
       </c>
-      <c r="E381" s="1" t="s">
+    </row>
+    <row r="382" spans="1:6">
+      <c r="C382" s="1" t="s">
         <v>1294</v>
       </c>
-    </row>
-    <row r="382" spans="1:6">
-      <c r="A382" s="1" t="s">
+      <c r="D382" s="1" t="s">
         <v>1295</v>
       </c>
-      <c r="B382" s="1" t="s">
+      <c r="E382" s="1" t="s">
         <v>1296</v>
       </c>
-      <c r="C382" s="1" t="s">
+    </row>
+    <row r="383" spans="1:6">
+      <c r="A383" s="1" t="s">
         <v>1297</v>
       </c>
-      <c r="D382" s="1" t="s">
+      <c r="B383" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="C383" s="1" t="s">
         <v>1298</v>
       </c>
-      <c r="E382" s="1" t="s">
+      <c r="D383" s="1" t="s">
         <v>1299</v>
       </c>
-      <c r="F382" s="1">
+      <c r="E383" s="1" t="s">
+        <v>1300</v>
+      </c>
+      <c r="F383" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="383" spans="1:6">
-      <c r="C383" s="1" t="s">
-        <v>1300</v>
-      </c>
-      <c r="D383" s="1" t="s">
+    <row r="384" spans="1:6">
+      <c r="C384" s="1" t="s">
         <v>1301</v>
       </c>
-      <c r="E383" s="1" t="s">
+      <c r="D384" s="1" t="s">
         <v>1302</v>
       </c>
-    </row>
-    <row r="384" spans="1:6">
-      <c r="A384" s="1" t="s">
+      <c r="E384" s="1" t="s">
         <v>1303</v>
       </c>
-      <c r="B384" s="1" t="s">
+    </row>
+    <row r="385" spans="1:6">
+      <c r="A385" s="1" t="s">
         <v>1304</v>
       </c>
-      <c r="C384" s="1" t="s">
+      <c r="B385" s="1" t="s">
         <v>1305</v>
       </c>
-      <c r="D384" s="1" t="s">
+      <c r="C385" s="1" t="s">
         <v>1306</v>
       </c>
-      <c r="E384" s="1" t="s">
+      <c r="D385" s="1" t="s">
         <v>1307</v>
       </c>
-      <c r="F384" s="1">
+      <c r="E385" s="1" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F385" s="1">
         <v>6</v>
-      </c>
-    </row>
-    <row r="385" spans="1:6">
-      <c r="C385" s="1" t="s">
-        <v>1308</v>
-      </c>
-      <c r="D385" s="1" t="s">
-        <v>1309</v>
-      </c>
-      <c r="E385" s="1" t="s">
-        <v>1310</v>
       </c>
     </row>
     <row r="386" spans="1:6">
       <c r="C386" s="1" t="s">
+        <v>1309</v>
+      </c>
+      <c r="D386" s="1" t="s">
+        <v>1310</v>
+      </c>
+      <c r="E386" s="1" t="s">
         <v>1311</v>
-      </c>
-      <c r="D386" s="1" t="s">
-        <v>1312</v>
-      </c>
-      <c r="E386" s="1" t="s">
-        <v>1313</v>
       </c>
     </row>
     <row r="387" spans="1:6">
       <c r="A387" s="1" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B387" s="1" t="s">
+        <v>1313</v>
+      </c>
+      <c r="C387" s="1" t="s">
         <v>1314</v>
       </c>
-      <c r="B387" s="1" t="s">
-        <v>927</v>
-      </c>
-      <c r="C387" s="1" t="s">
+      <c r="D387" s="1" t="s">
         <v>1315</v>
-      </c>
-      <c r="D387" s="1" t="s">
-        <v>1314</v>
       </c>
       <c r="E387" s="1" t="s">
         <v>1316</v>
       </c>
       <c r="F387" s="1">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="388" spans="1:6">
@@ -11060,65 +11261,65 @@
       </c>
     </row>
     <row r="389" spans="1:6">
-      <c r="A389" s="1" t="s">
+      <c r="C389" s="1" t="s">
         <v>1320</v>
       </c>
-      <c r="B389" s="1" t="s">
+      <c r="D389" s="1" t="s">
         <v>1321</v>
       </c>
-      <c r="C389" s="1" t="s">
+      <c r="E389" s="1" t="s">
         <v>1322</v>
-      </c>
-      <c r="D389" s="1" t="s">
-        <v>1323</v>
-      </c>
-      <c r="E389" s="1" t="s">
-        <v>1324</v>
-      </c>
-      <c r="F389" s="1">
-        <v>5</v>
       </c>
     </row>
     <row r="390" spans="1:6">
       <c r="A390" s="1" t="s">
+        <v>1323</v>
+      </c>
+      <c r="B390" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C390" s="1" t="s">
+        <v>1324</v>
+      </c>
+      <c r="D390" s="1" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E390" s="1" t="s">
         <v>1325</v>
       </c>
-      <c r="B390" s="1" t="s">
-        <v>1326</v>
-      </c>
-      <c r="C390" s="1" t="s">
-        <v>1327</v>
-      </c>
-      <c r="D390" s="1" t="s">
-        <v>1325</v>
-      </c>
-      <c r="E390" s="1" t="s">
-        <v>1328</v>
-      </c>
       <c r="F390" s="1">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="391" spans="1:6">
       <c r="C391" s="1" t="s">
+        <v>1326</v>
+      </c>
+      <c r="D391" s="1" t="s">
+        <v>1327</v>
+      </c>
+      <c r="E391" s="1" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="392" spans="1:6">
+      <c r="A392" s="1" t="s">
         <v>1329</v>
       </c>
-      <c r="D391" s="1" t="s">
+      <c r="B392" s="1" t="s">
         <v>1330</v>
       </c>
-      <c r="E391" s="1" t="s">
+      <c r="C392" s="1" t="s">
         <v>1331</v>
       </c>
-    </row>
-    <row r="392" spans="1:6">
-      <c r="C392" s="1" t="s">
+      <c r="D392" s="1" t="s">
         <v>1332</v>
       </c>
-      <c r="D392" s="1" t="s">
+      <c r="E392" s="1" t="s">
         <v>1333</v>
       </c>
-      <c r="E392" s="1" t="s">
-        <v>706</v>
+      <c r="F392" s="1">
+        <v>5</v>
       </c>
     </row>
     <row r="393" spans="1:6">
@@ -11135,7 +11336,7 @@
         <v>1334</v>
       </c>
       <c r="E393" s="1" t="s">
-        <v>1335</v>
+        <v>1337</v>
       </c>
       <c r="F393" s="1">
         <v>8</v>
@@ -11143,75 +11344,75 @@
     </row>
     <row r="394" spans="1:6">
       <c r="C394" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="D394" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="E394" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="395" spans="1:6">
-      <c r="A395" s="1" t="s">
-        <v>1340</v>
-      </c>
-      <c r="B395" s="1" t="s">
+      <c r="C395" s="1" t="s">
         <v>1341</v>
       </c>
-      <c r="C395" s="1" t="s">
+      <c r="D395" s="1" t="s">
         <v>1342</v>
       </c>
-      <c r="D395" s="1" t="s">
-        <v>1340</v>
-      </c>
       <c r="E395" s="1" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="396" spans="1:6">
+      <c r="A396" s="1" t="s">
         <v>1343</v>
       </c>
-      <c r="F395" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="396" spans="1:6">
+      <c r="B396" s="1" t="s">
+        <v>1344</v>
+      </c>
       <c r="C396" s="1" t="s">
+        <v>1345</v>
+      </c>
+      <c r="D396" s="1" t="s">
+        <v>1343</v>
+      </c>
+      <c r="E396" s="1" t="s">
         <v>1344</v>
       </c>
-      <c r="D396" s="1" t="s">
-        <v>1345</v>
-      </c>
-      <c r="E396" s="1" t="s">
-        <v>1346</v>
+      <c r="F396" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="397" spans="1:6">
       <c r="C397" s="1" t="s">
+        <v>1346</v>
+      </c>
+      <c r="D397" s="1" t="s">
         <v>1347</v>
       </c>
-      <c r="D397" s="1" t="s">
+      <c r="E397" s="1" t="s">
         <v>1348</v>
-      </c>
-      <c r="E397" s="1" t="s">
-        <v>1349</v>
       </c>
     </row>
     <row r="398" spans="1:6">
       <c r="A398" s="1" t="s">
+        <v>1349</v>
+      </c>
+      <c r="B398" s="1" t="s">
         <v>1350</v>
-      </c>
-      <c r="B398" s="1" t="s">
-        <v>765</v>
       </c>
       <c r="C398" s="1" t="s">
         <v>1351</v>
       </c>
       <c r="D398" s="1" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="E398" s="1" t="s">
         <v>1352</v>
       </c>
       <c r="F398" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="399" spans="1:6">
@@ -11241,95 +11442,92 @@
         <v>1359</v>
       </c>
       <c r="B401" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="C401" s="1" t="s">
         <v>1360</v>
-      </c>
-      <c r="C401" s="1" t="s">
-        <v>1361</v>
       </c>
       <c r="D401" s="1" t="s">
         <v>1359</v>
       </c>
       <c r="E401" s="1" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="F401" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="402" spans="1:6">
       <c r="C402" s="1" t="s">
+        <v>1362</v>
+      </c>
+      <c r="D402" s="1" t="s">
         <v>1363</v>
       </c>
-      <c r="D402" s="1" t="s">
+      <c r="E402" s="1" t="s">
         <v>1364</v>
-      </c>
-      <c r="E402" s="1" t="s">
-        <v>1365</v>
       </c>
     </row>
     <row r="403" spans="1:6">
       <c r="C403" s="1" t="s">
+        <v>1365</v>
+      </c>
+      <c r="D403" s="1" t="s">
         <v>1366</v>
       </c>
-      <c r="D403" s="1" t="s">
+      <c r="E403" s="1" t="s">
         <v>1367</v>
-      </c>
-      <c r="E403" s="1" t="s">
-        <v>1368</v>
       </c>
     </row>
     <row r="404" spans="1:6">
       <c r="A404" s="1" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B404" s="1" t="s">
         <v>1369</v>
       </c>
-      <c r="B404" s="1" t="s">
+      <c r="C404" s="1" t="s">
         <v>1370</v>
       </c>
-      <c r="C404" s="1" t="s">
+      <c r="D404" s="1" t="s">
+        <v>1368</v>
+      </c>
+      <c r="E404" s="1" t="s">
         <v>1371</v>
       </c>
-      <c r="D404" s="1" t="s">
-        <v>1372</v>
-      </c>
-      <c r="E404" s="1" t="s">
-        <v>1373</v>
-      </c>
       <c r="F404" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="405" spans="1:6">
       <c r="C405" s="1" t="s">
+        <v>1372</v>
+      </c>
+      <c r="D405" s="1" t="s">
+        <v>1373</v>
+      </c>
+      <c r="E405" s="1" t="s">
         <v>1374</v>
       </c>
-      <c r="D405" s="1" t="s">
+    </row>
+    <row r="406" spans="1:6">
+      <c r="C406" s="1" t="s">
         <v>1375</v>
       </c>
-      <c r="E405" s="1" t="s">
+      <c r="D406" s="1" t="s">
         <v>1376</v>
       </c>
-    </row>
-    <row r="406" spans="1:6">
-      <c r="A406" s="1" t="s">
+      <c r="E406" s="1" t="s">
         <v>1377</v>
       </c>
-      <c r="B406" s="1" t="s">
+    </row>
+    <row r="407" spans="1:6">
+      <c r="A407" s="1" t="s">
         <v>1378</v>
       </c>
-      <c r="C406" s="1" t="s">
+      <c r="B407" s="1" t="s">
         <v>1379</v>
       </c>
-      <c r="D406" s="1" t="s">
-        <v>1377</v>
-      </c>
-      <c r="E406" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="F406" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="407" spans="1:6">
       <c r="C407" s="1" t="s">
         <v>1380</v>
       </c>
@@ -11338,6 +11536,9 @@
       </c>
       <c r="E407" s="1" t="s">
         <v>1382</v>
+      </c>
+      <c r="F407" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="408" spans="1:6">
@@ -11362,170 +11563,170 @@
         <v>1388</v>
       </c>
       <c r="D409" s="1" t="s">
+        <v>1386</v>
+      </c>
+      <c r="E409" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F409" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="410" spans="1:6">
+      <c r="C410" s="1" t="s">
         <v>1389</v>
       </c>
-      <c r="E409" s="1" t="s">
+      <c r="D410" s="1" t="s">
         <v>1390</v>
       </c>
-      <c r="F409" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="410" spans="1:6">
-      <c r="A410" s="1" t="s">
+      <c r="E410" s="1" t="s">
         <v>1391</v>
-      </c>
-      <c r="B410" s="1" t="s">
-        <v>1392</v>
-      </c>
-      <c r="C410" s="1" t="s">
-        <v>1393</v>
-      </c>
-      <c r="D410" s="1" t="s">
-        <v>1394</v>
-      </c>
-      <c r="E410" s="1" t="s">
-        <v>1395</v>
-      </c>
-      <c r="F410" s="1">
-        <v>11</v>
       </c>
     </row>
     <row r="411" spans="1:6">
       <c r="C411" s="1" t="s">
+        <v>1392</v>
+      </c>
+      <c r="D411" s="1" t="s">
+        <v>1393</v>
+      </c>
+      <c r="E411" s="1" t="s">
+        <v>1394</v>
+      </c>
+    </row>
+    <row r="412" spans="1:6">
+      <c r="A412" s="1" t="s">
+        <v>1395</v>
+      </c>
+      <c r="B412" s="1" t="s">
         <v>1396</v>
       </c>
-      <c r="D411" s="1" t="s">
+      <c r="C412" s="1" t="s">
         <v>1397</v>
       </c>
-      <c r="E411" s="1" t="s">
+      <c r="D412" s="1" t="s">
         <v>1398</v>
       </c>
-    </row>
-    <row r="412" spans="1:6">
-      <c r="C412" s="1" t="s">
+      <c r="E412" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="D412" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="E412" s="1" t="s">
-        <v>1401</v>
+      <c r="F412" s="1">
+        <v>10</v>
       </c>
     </row>
     <row r="413" spans="1:6">
       <c r="A413" s="1" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B413" s="1" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C413" s="1" t="s">
         <v>1402</v>
       </c>
-      <c r="B413" s="1" t="s">
+      <c r="D413" s="1" t="s">
         <v>1403</v>
       </c>
-      <c r="C413" s="1" t="s">
+      <c r="E413" s="1" t="s">
         <v>1404</v>
       </c>
-      <c r="D413" s="1" t="s">
-        <v>1402</v>
-      </c>
-      <c r="E413" s="1" t="s">
-        <v>1405</v>
-      </c>
       <c r="F413" s="1">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="414" spans="1:6">
       <c r="C414" s="1" t="s">
-        <v>263</v>
+        <v>1405</v>
       </c>
       <c r="D414" s="1" t="s">
-        <v>264</v>
+        <v>1406</v>
       </c>
       <c r="E414" s="1" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="415" spans="1:6">
       <c r="C415" s="1" t="s">
-        <v>1083</v>
+        <v>1408</v>
       </c>
       <c r="D415" s="1" t="s">
-        <v>1084</v>
+        <v>1409</v>
       </c>
       <c r="E415" s="1" t="s">
-        <v>1407</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="416" spans="1:6">
+      <c r="A416" s="1" t="s">
+        <v>1411</v>
+      </c>
+      <c r="B416" s="1" t="s">
+        <v>1412</v>
+      </c>
       <c r="C416" s="1" t="s">
-        <v>1100</v>
+        <v>1413</v>
       </c>
       <c r="D416" s="1" t="s">
-        <v>1101</v>
+        <v>1411</v>
       </c>
       <c r="E416" s="1" t="s">
-        <v>1085</v>
+        <v>1414</v>
+      </c>
+      <c r="F416" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="417" spans="1:6">
-      <c r="A417" s="1" t="s">
-        <v>1408</v>
-      </c>
-      <c r="B417" s="1" t="s">
-        <v>1409</v>
-      </c>
       <c r="C417" s="1" t="s">
-        <v>1410</v>
+        <v>263</v>
       </c>
       <c r="D417" s="1" t="s">
-        <v>1408</v>
+        <v>264</v>
       </c>
       <c r="E417" s="1" t="s">
-        <v>1411</v>
-      </c>
-      <c r="F417" s="1">
-        <v>5</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="418" spans="1:6">
-      <c r="A418" s="1" t="s">
-        <v>1412</v>
-      </c>
-      <c r="B418" s="1" t="s">
-        <v>1413</v>
-      </c>
       <c r="C418" s="1" t="s">
-        <v>1414</v>
+        <v>1086</v>
       </c>
       <c r="D418" s="1" t="s">
-        <v>1412</v>
+        <v>1087</v>
       </c>
       <c r="E418" s="1" t="s">
-        <v>1415</v>
-      </c>
-      <c r="F418" s="1">
-        <v>7</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="419" spans="1:6">
       <c r="C419" s="1" t="s">
-        <v>1416</v>
+        <v>1103</v>
       </c>
       <c r="D419" s="1" t="s">
+        <v>1104</v>
+      </c>
+      <c r="E419" s="1" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="420" spans="1:6">
+      <c r="A420" s="1" t="s">
         <v>1417</v>
       </c>
-      <c r="E419" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="420" spans="1:6">
+      <c r="B420" s="1" t="s">
+        <v>1418</v>
+      </c>
       <c r="C420" s="1" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="D420" s="1" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="E420" s="1" t="s">
         <v>1420</v>
+      </c>
+      <c r="F420" s="1">
+        <v>5</v>
       </c>
     </row>
     <row r="421" spans="1:6">
@@ -11539,160 +11740,157 @@
         <v>1423</v>
       </c>
       <c r="D421" s="1" t="s">
+        <v>1421</v>
+      </c>
+      <c r="E421" s="1" t="s">
         <v>1424</v>
       </c>
-      <c r="E421" s="1" t="s">
+      <c r="F421" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="422" spans="1:6">
+      <c r="C422" s="1" t="s">
         <v>1425</v>
       </c>
-      <c r="F421" s="1">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="422" spans="1:6">
-      <c r="A422" s="1" t="s">
+      <c r="D422" s="1" t="s">
         <v>1426</v>
       </c>
-      <c r="B422" s="1" t="s">
-        <v>1427</v>
-      </c>
-      <c r="C422" s="1" t="s">
-        <v>1428</v>
-      </c>
-      <c r="D422" s="1" t="s">
-        <v>1429</v>
-      </c>
       <c r="E422" s="1" t="s">
-        <v>1430</v>
-      </c>
-      <c r="F422" s="1">
-        <v>9</v>
+        <v>333</v>
       </c>
     </row>
     <row r="423" spans="1:6">
       <c r="C423" s="1" t="s">
+        <v>1427</v>
+      </c>
+      <c r="D423" s="1" t="s">
+        <v>1428</v>
+      </c>
+      <c r="E423" s="1" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="424" spans="1:6">
+      <c r="A424" s="1" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B424" s="1" t="s">
         <v>1431</v>
       </c>
-      <c r="D423" s="1" t="s">
+      <c r="C424" s="1" t="s">
         <v>1432</v>
       </c>
-      <c r="E423" s="1" t="s">
+      <c r="D424" s="1" t="s">
         <v>1433</v>
       </c>
-    </row>
-    <row r="424" spans="1:6">
-      <c r="C424" s="1" t="s">
+      <c r="E424" s="1" t="s">
         <v>1434</v>
       </c>
-      <c r="D424" s="1" t="s">
-        <v>1435</v>
-      </c>
-      <c r="E424" s="1" t="s">
-        <v>1436</v>
+      <c r="F424" s="1">
+        <v>19</v>
       </c>
     </row>
     <row r="425" spans="1:6">
       <c r="A425" s="1" t="s">
+        <v>1435</v>
+      </c>
+      <c r="B425" s="1" t="s">
+        <v>1436</v>
+      </c>
+      <c r="C425" s="1" t="s">
         <v>1437</v>
       </c>
-      <c r="B425" s="1" t="s">
+      <c r="D425" s="1" t="s">
         <v>1438</v>
       </c>
-      <c r="C425" s="1" t="s">
+      <c r="E425" s="1" t="s">
         <v>1439</v>
       </c>
-      <c r="D425" s="1" t="s">
-        <v>1437</v>
-      </c>
-      <c r="E425" s="1" t="s">
-        <v>1440</v>
-      </c>
       <c r="F425" s="1">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="426" spans="1:6">
       <c r="C426" s="1" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D426" s="1" t="s">
         <v>1441</v>
       </c>
-      <c r="D426" s="1" t="s">
+      <c r="E426" s="1" t="s">
         <v>1442</v>
       </c>
-      <c r="E426" s="1" t="s">
+    </row>
+    <row r="427" spans="1:6">
+      <c r="C427" s="1" t="s">
         <v>1443</v>
       </c>
-    </row>
-    <row r="427" spans="1:6">
-      <c r="A427" s="1" t="s">
+      <c r="D427" s="1" t="s">
         <v>1444</v>
       </c>
-      <c r="B427" s="1" t="s">
+      <c r="E427" s="1" t="s">
         <v>1445</v>
-      </c>
-      <c r="C427" s="1" t="s">
-        <v>1446</v>
-      </c>
-      <c r="D427" s="1" t="s">
-        <v>1447</v>
-      </c>
-      <c r="E427" s="1" t="s">
-        <v>1448</v>
-      </c>
-      <c r="F427" s="1">
-        <v>11</v>
       </c>
     </row>
     <row r="428" spans="1:6">
       <c r="A428" s="1" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B428" s="1" t="s">
+        <v>1447</v>
+      </c>
+      <c r="C428" s="1" t="s">
+        <v>1448</v>
+      </c>
+      <c r="D428" s="1" t="s">
+        <v>1446</v>
+      </c>
+      <c r="E428" s="1" t="s">
         <v>1449</v>
       </c>
-      <c r="B428" s="1" t="s">
-        <v>1273</v>
-      </c>
-      <c r="C428" s="1" t="s">
-        <v>1450</v>
-      </c>
-      <c r="D428" s="1" t="s">
-        <v>1451</v>
-      </c>
-      <c r="E428" s="1" t="s">
-        <v>1452</v>
-      </c>
       <c r="F428" s="1">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="429" spans="1:6">
       <c r="C429" s="1" t="s">
-        <v>1271</v>
+        <v>1450</v>
       </c>
       <c r="D429" s="1" t="s">
-        <v>1272</v>
+        <v>1451</v>
       </c>
       <c r="E429" s="1" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="430" spans="1:6">
       <c r="A430" s="1" t="s">
+        <v>1453</v>
+      </c>
+      <c r="B430" s="1" t="s">
         <v>1454</v>
       </c>
-      <c r="B430" s="1" t="s">
+      <c r="C430" s="1" t="s">
         <v>1455</v>
       </c>
-      <c r="C430" s="1" t="s">
+      <c r="D430" s="1" t="s">
         <v>1456</v>
       </c>
-      <c r="D430" s="1" t="s">
+      <c r="E430" s="1" t="s">
         <v>1457</v>
       </c>
-      <c r="E430" s="1" t="s">
+      <c r="F430" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="431" spans="1:6">
+      <c r="A431" s="1" t="s">
         <v>1458</v>
       </c>
-      <c r="F430" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="431" spans="1:6">
+      <c r="B431" s="1" t="s">
+        <v>1282</v>
+      </c>
       <c r="C431" s="1" t="s">
         <v>1459</v>
       </c>
@@ -11702,19 +11900,28 @@
       <c r="E431" s="1" t="s">
         <v>1461</v>
       </c>
+      <c r="F431" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="432" spans="1:6">
       <c r="C432" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D432" s="1" t="s">
+        <v>1281</v>
+      </c>
+      <c r="E432" s="1" t="s">
         <v>1462</v>
       </c>
-      <c r="D432" s="1" t="s">
+    </row>
+    <row r="433" spans="1:6">
+      <c r="A433" s="1" t="s">
         <v>1463</v>
       </c>
-      <c r="E432" s="1" t="s">
+      <c r="B433" s="1" t="s">
         <v>1464</v>
       </c>
-    </row>
-    <row r="433" spans="1:6">
       <c r="C433" s="1" t="s">
         <v>1465</v>
       </c>
@@ -11724,116 +11931,104 @@
       <c r="E433" s="1" t="s">
         <v>1467</v>
       </c>
+      <c r="F433" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="434" spans="1:6">
-      <c r="A434" s="1" t="s">
+      <c r="C434" s="1" t="s">
         <v>1468</v>
       </c>
-      <c r="B434" s="1" t="s">
+      <c r="D434" s="1" t="s">
         <v>1469</v>
       </c>
-      <c r="C434" s="1" t="s">
+      <c r="E434" s="1" t="s">
         <v>1470</v>
-      </c>
-      <c r="D434" s="1" t="s">
-        <v>1471</v>
-      </c>
-      <c r="E434" s="1" t="s">
-        <v>1472</v>
-      </c>
-      <c r="F434">
-        <v>5</v>
       </c>
     </row>
     <row r="435" spans="1:6">
       <c r="C435" s="1" t="s">
+        <v>1471</v>
+      </c>
+      <c r="D435" s="1" t="s">
+        <v>1472</v>
+      </c>
+      <c r="E435" s="1" t="s">
+        <v>1473</v>
+      </c>
+    </row>
+    <row r="436" spans="1:6">
+      <c r="C436" s="1" t="s">
+        <v>1474</v>
+      </c>
+      <c r="D436" s="1" t="s">
+        <v>1475</v>
+      </c>
+      <c r="E436" s="1" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="437" spans="1:6">
+      <c r="A437" s="1" t="s">
+        <v>1477</v>
+      </c>
+      <c r="B437" s="1" t="s">
+        <v>1478</v>
+      </c>
+      <c r="C437" s="1" t="s">
+        <v>1479</v>
+      </c>
+      <c r="D437" s="1" t="s">
+        <v>1480</v>
+      </c>
+      <c r="E437" s="1" t="s">
+        <v>1481</v>
+      </c>
+      <c r="F437">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="438" spans="1:6">
+      <c r="C438" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="D435" s="1" t="s">
-        <v>1473</v>
-      </c>
-      <c r="E435" s="1" t="s">
+      <c r="D438" s="1" t="s">
+        <v>1482</v>
+      </c>
+      <c r="E438" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="F435"/>
-    </row>
-    <row r="436" spans="1:6">
-      <c r="A436" s="2"/>
-      <c r="B436" s="2"/>
-      <c r="C436" s="2" t="s">
-        <v>1474</v>
-      </c>
-      <c r="D436" s="2" t="s">
-        <v>1475</v>
-      </c>
-      <c r="E436" s="2" t="s">
-        <v>1476</v>
-      </c>
-      <c r="F436" s="2"/>
-    </row>
-    <row r="437" spans="1:6">
-      <c r="A437" s="2" t="s">
-        <v>1477</v>
-      </c>
-      <c r="B437" s="2" t="s">
-        <v>1478</v>
-      </c>
-      <c r="C437" s="2" t="s">
-        <v>1479</v>
-      </c>
-      <c r="D437" s="2" t="s">
-        <v>1480</v>
-      </c>
-      <c r="E437" s="2" t="s">
-        <v>1481</v>
-      </c>
-      <c r="F437" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="438" spans="1:6">
-      <c r="A438" s="2"/>
-      <c r="B438" s="2"/>
-      <c r="C438" s="2" t="s">
-        <v>1482</v>
-      </c>
-      <c r="D438" s="2" t="s">
-        <v>1483</v>
-      </c>
-      <c r="E438" s="2" t="s">
-        <v>1484</v>
-      </c>
-      <c r="F438" s="2"/>
+      <c r="F438"/>
     </row>
     <row r="439" spans="1:6">
       <c r="A439" s="2"/>
       <c r="B439" s="2"/>
       <c r="C439" s="2" t="s">
+        <v>1483</v>
+      </c>
+      <c r="D439" s="2" t="s">
+        <v>1484</v>
+      </c>
+      <c r="E439" s="2" t="s">
         <v>1485</v>
-      </c>
-      <c r="D439" s="2" t="s">
-        <v>1486</v>
-      </c>
-      <c r="E439" s="2" t="s">
-        <v>1487</v>
       </c>
       <c r="F439" s="2"/>
     </row>
     <row r="440" spans="1:6">
       <c r="A440" s="2" t="s">
+        <v>1486</v>
+      </c>
+      <c r="B440" s="2" t="s">
+        <v>1487</v>
+      </c>
+      <c r="C440" s="2" t="s">
         <v>1488</v>
       </c>
-      <c r="B440" s="2" t="s">
+      <c r="D440" s="2" t="s">
         <v>1489</v>
       </c>
-      <c r="C440" s="2" t="s">
+      <c r="E440" s="2" t="s">
         <v>1490</v>
-      </c>
-      <c r="D440" s="2" t="s">
-        <v>1491</v>
-      </c>
-      <c r="E440" s="2" t="s">
-        <v>1492</v>
       </c>
       <c r="F440" s="2">
         <v>9</v>
@@ -11843,197 +12038,197 @@
       <c r="A441" s="2"/>
       <c r="B441" s="2"/>
       <c r="C441" s="2" t="s">
+        <v>1491</v>
+      </c>
+      <c r="D441" s="2" t="s">
+        <v>1492</v>
+      </c>
+      <c r="E441" s="2" t="s">
         <v>1493</v>
       </c>
-      <c r="D441" s="2" t="s">
+      <c r="F441" s="2"/>
+    </row>
+    <row r="442" spans="1:6">
+      <c r="A442" s="2"/>
+      <c r="B442" s="2"/>
+      <c r="C442" s="2" t="s">
         <v>1494</v>
       </c>
-      <c r="E441" s="2" t="s">
+      <c r="D442" s="2" t="s">
         <v>1495</v>
       </c>
-      <c r="F441" s="2"/>
-    </row>
-    <row r="442" spans="1:6">
-      <c r="A442" s="2" t="s">
+      <c r="E442" s="2" t="s">
         <v>1496</v>
       </c>
-      <c r="B442" s="2" t="s">
-        <v>1497</v>
-      </c>
-      <c r="C442" s="2" t="s">
-        <v>1498</v>
-      </c>
-      <c r="D442" s="2" t="s">
-        <v>1499</v>
-      </c>
-      <c r="E442" s="2" t="s">
-        <v>1500</v>
-      </c>
-      <c r="F442" s="2">
-        <v>7</v>
-      </c>
+      <c r="F442" s="2"/>
     </row>
     <row r="443" spans="1:6">
       <c r="A443" s="2" t="s">
+        <v>1497</v>
+      </c>
+      <c r="B443" s="2" t="s">
+        <v>1498</v>
+      </c>
+      <c r="C443" s="2" t="s">
+        <v>1499</v>
+      </c>
+      <c r="D443" s="2" t="s">
+        <v>1500</v>
+      </c>
+      <c r="E443" s="2" t="s">
         <v>1501</v>
       </c>
-      <c r="B443" s="2" t="s">
-        <v>1502</v>
-      </c>
-      <c r="C443" s="2" t="s">
-        <v>1503</v>
-      </c>
-      <c r="D443" s="2" t="s">
-        <v>1504</v>
-      </c>
-      <c r="E443" s="2" t="s">
-        <v>1505</v>
-      </c>
       <c r="F443" s="2">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="444" spans="1:6">
       <c r="A444" s="2"/>
       <c r="B444" s="2"/>
       <c r="C444" s="2" t="s">
-        <v>1506</v>
+        <v>1502</v>
       </c>
       <c r="D444" s="2" t="s">
-        <v>1507</v>
+        <v>1503</v>
       </c>
       <c r="E444" s="2" t="s">
-        <v>1508</v>
+        <v>1504</v>
       </c>
       <c r="F444" s="2"/>
     </row>
     <row r="445" spans="1:6">
       <c r="A445" s="2" t="s">
+        <v>1505</v>
+      </c>
+      <c r="B445" s="2" t="s">
+        <v>1506</v>
+      </c>
+      <c r="C445" s="2" t="s">
+        <v>1507</v>
+      </c>
+      <c r="D445" s="2" t="s">
+        <v>1508</v>
+      </c>
+      <c r="E445" s="2" t="s">
         <v>1509</v>
       </c>
-      <c r="B445" s="2" t="s">
+      <c r="F445" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="446" spans="1:6">
+      <c r="A446" s="2" t="s">
         <v>1510</v>
       </c>
-      <c r="C445" s="2" t="s">
+      <c r="B446" s="2" t="s">
         <v>1511</v>
       </c>
-      <c r="D445" s="2" t="s">
+      <c r="C446" s="2" t="s">
         <v>1512</v>
       </c>
-      <c r="E445" s="2" t="s">
+      <c r="D446" s="2" t="s">
         <v>1513</v>
       </c>
-      <c r="F445" s="2">
+      <c r="E446" s="2" t="s">
+        <v>1514</v>
+      </c>
+      <c r="F446" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="447" spans="1:6">
+      <c r="A447" s="2"/>
+      <c r="B447" s="2"/>
+      <c r="C447" s="2" t="s">
+        <v>1515</v>
+      </c>
+      <c r="D447" s="2" t="s">
+        <v>1516</v>
+      </c>
+      <c r="E447" s="2" t="s">
+        <v>1517</v>
+      </c>
+      <c r="F447" s="2"/>
+    </row>
+    <row r="448" spans="1:6">
+      <c r="A448" s="2" t="s">
+        <v>1518</v>
+      </c>
+      <c r="B448" s="2" t="s">
+        <v>1519</v>
+      </c>
+      <c r="C448" s="2" t="s">
+        <v>1520</v>
+      </c>
+      <c r="D448" s="2" t="s">
+        <v>1521</v>
+      </c>
+      <c r="E448" s="2" t="s">
+        <v>1522</v>
+      </c>
+      <c r="F448" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="446" spans="1:6">
-      <c r="A446" s="2"/>
-      <c r="B446" s="2"/>
-      <c r="C446" s="2" t="s">
-        <v>1514</v>
-      </c>
-      <c r="D446" s="2" t="s">
-        <v>1515</v>
-      </c>
-      <c r="E446" s="2" t="s">
-        <v>1516</v>
-      </c>
-      <c r="F446" s="2"/>
-    </row>
-    <row r="447" spans="1:6">
-      <c r="A447" s="2" t="s">
-        <v>1517</v>
-      </c>
-      <c r="B447" s="2" t="s">
-        <v>1518</v>
-      </c>
-      <c r="C447" s="2" t="s">
-        <v>1519</v>
-      </c>
-      <c r="D447" s="2" t="s">
-        <v>1520</v>
-      </c>
-      <c r="E447" s="2" t="s">
-        <v>1521</v>
-      </c>
-      <c r="F447" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="448" spans="1:6">
-      <c r="A448" s="2"/>
-      <c r="B448" s="2"/>
-      <c r="C448" s="2" t="s">
-        <v>1522</v>
-      </c>
-      <c r="D448" s="2" t="s">
-        <v>1523</v>
-      </c>
-      <c r="E448" s="2" t="s">
-        <v>1524</v>
-      </c>
-      <c r="F448" s="2"/>
     </row>
     <row r="449" spans="1:6">
       <c r="A449" s="2"/>
       <c r="B449" s="2"/>
       <c r="C449" s="2" t="s">
+        <v>1523</v>
+      </c>
+      <c r="D449" s="2" t="s">
+        <v>1524</v>
+      </c>
+      <c r="E449" s="2" t="s">
         <v>1525</v>
       </c>
-      <c r="D449" s="2" t="s">
+      <c r="F449" s="2"/>
+    </row>
+    <row r="450" spans="1:6">
+      <c r="A450" s="2" t="s">
         <v>1526</v>
       </c>
-      <c r="E449" s="2" t="s">
+      <c r="B450" s="2" t="s">
         <v>1527</v>
       </c>
-      <c r="F449" s="2"/>
-    </row>
-    <row r="450" spans="1:6">
-      <c r="A450" s="2"/>
-      <c r="B450" s="2"/>
       <c r="C450" s="2" t="s">
-        <v>212</v>
+        <v>1528</v>
       </c>
       <c r="D450" s="2" t="s">
-        <v>213</v>
+        <v>1529</v>
       </c>
       <c r="E450" s="2" t="s">
-        <v>1528</v>
-      </c>
-      <c r="F450" s="2"/>
+        <v>1530</v>
+      </c>
+      <c r="F450" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="451" spans="1:6">
-      <c r="A451" s="2" t="s">
-        <v>1529</v>
-      </c>
-      <c r="B451" s="2" t="s">
-        <v>1530</v>
-      </c>
+      <c r="A451" s="2"/>
+      <c r="B451" s="2"/>
       <c r="C451" s="2" t="s">
-        <v>1522</v>
+        <v>1531</v>
       </c>
       <c r="D451" s="2" t="s">
-        <v>1523</v>
+        <v>1532</v>
       </c>
       <c r="E451" s="2" t="s">
-        <v>1524</v>
-      </c>
-      <c r="F451" s="2">
-        <v>9</v>
-      </c>
+        <v>1533</v>
+      </c>
+      <c r="F451" s="2"/>
     </row>
     <row r="452" spans="1:6">
       <c r="A452" s="2"/>
       <c r="B452" s="2"/>
       <c r="C452" s="2" t="s">
-        <v>1531</v>
+        <v>1534</v>
       </c>
       <c r="D452" s="2" t="s">
-        <v>1532</v>
+        <v>1535</v>
       </c>
       <c r="E452" s="2" t="s">
-        <v>1533</v>
+        <v>1536</v>
       </c>
       <c r="F452" s="2"/>
     </row>
@@ -12041,31 +12236,31 @@
       <c r="A453" s="2"/>
       <c r="B453" s="2"/>
       <c r="C453" s="2" t="s">
-        <v>1534</v>
+        <v>212</v>
       </c>
       <c r="D453" s="2" t="s">
-        <v>1535</v>
+        <v>213</v>
       </c>
       <c r="E453" s="2" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="F453" s="2"/>
     </row>
     <row r="454" spans="1:6">
       <c r="A454" s="2" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="B454" s="2" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="C454" s="2" t="s">
-        <v>974</v>
+        <v>1531</v>
       </c>
       <c r="D454" s="2" t="s">
-        <v>975</v>
+        <v>1532</v>
       </c>
       <c r="E454" s="2" t="s">
-        <v>976</v>
+        <v>1533</v>
       </c>
       <c r="F454" s="2">
         <v>9</v>
@@ -12075,13 +12270,13 @@
       <c r="A455" s="2"/>
       <c r="B455" s="2"/>
       <c r="C455" s="2" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D455" s="2" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="E455" s="2" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="F455" s="2"/>
     </row>
@@ -12089,75 +12284,75 @@
       <c r="A456" s="2"/>
       <c r="B456" s="2"/>
       <c r="C456" s="2" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D456" s="2" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="E456" s="2" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="F456" s="2"/>
     </row>
     <row r="457" spans="1:6">
-      <c r="A457" s="2"/>
-      <c r="B457" s="2"/>
+      <c r="A457" s="2" t="s">
+        <v>1546</v>
+      </c>
+      <c r="B457" s="2" t="s">
+        <v>1547</v>
+      </c>
       <c r="C457" s="2" t="s">
-        <v>1493</v>
+        <v>974</v>
       </c>
       <c r="D457" s="2" t="s">
-        <v>1494</v>
+        <v>975</v>
       </c>
       <c r="E457" s="2" t="s">
-        <v>1495</v>
-      </c>
-      <c r="F457" s="2"/>
+        <v>976</v>
+      </c>
+      <c r="F457" s="2">
+        <v>9</v>
+      </c>
     </row>
     <row r="458" spans="1:6">
       <c r="A458" s="2"/>
       <c r="B458" s="2"/>
       <c r="C458" s="2" t="s">
-        <v>1545</v>
+        <v>1548</v>
       </c>
       <c r="D458" s="2" t="s">
-        <v>1546</v>
+        <v>1549</v>
       </c>
       <c r="E458" s="2" t="s">
-        <v>1547</v>
+        <v>1550</v>
       </c>
       <c r="F458" s="2"/>
     </row>
     <row r="459" spans="1:6">
-      <c r="A459" s="2" t="s">
-        <v>1548</v>
-      </c>
-      <c r="B459" s="2" t="s">
-        <v>1549</v>
-      </c>
+      <c r="A459" s="2"/>
+      <c r="B459" s="2"/>
       <c r="C459" s="2" t="s">
-        <v>1108</v>
+        <v>1551</v>
       </c>
       <c r="D459" s="2" t="s">
-        <v>1109</v>
+        <v>1552</v>
       </c>
       <c r="E459" s="2" t="s">
-        <v>1110</v>
-      </c>
-      <c r="F459" s="2">
-        <v>12</v>
-      </c>
+        <v>1553</v>
+      </c>
+      <c r="F459" s="2"/>
     </row>
     <row r="460" spans="1:6">
       <c r="A460" s="2"/>
       <c r="B460" s="2"/>
       <c r="C460" s="2" t="s">
-        <v>1550</v>
+        <v>1502</v>
       </c>
       <c r="D460" s="2" t="s">
-        <v>1551</v>
+        <v>1503</v>
       </c>
       <c r="E460" s="2" t="s">
-        <v>1552</v>
+        <v>1504</v>
       </c>
       <c r="F460" s="2"/>
     </row>
@@ -12165,29 +12360,35 @@
       <c r="A461" s="2"/>
       <c r="B461" s="2"/>
       <c r="C461" s="2" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="D461" s="2" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="E461" s="2" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="F461" s="2"/>
     </row>
     <row r="462" spans="1:6">
-      <c r="A462" s="2"/>
-      <c r="B462" s="2"/>
+      <c r="A462" s="2" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B462" s="2" t="s">
+        <v>1558</v>
+      </c>
       <c r="C462" s="2" t="s">
-        <v>1556</v>
+        <v>1111</v>
       </c>
       <c r="D462" s="2" t="s">
-        <v>1557</v>
+        <v>1112</v>
       </c>
       <c r="E462" s="2" t="s">
-        <v>1558</v>
-      </c>
-      <c r="F462" s="2"/>
+        <v>1113</v>
+      </c>
+      <c r="F462" s="2">
+        <v>12</v>
+      </c>
     </row>
     <row r="463" spans="1:6">
       <c r="A463" s="2"/>
@@ -12246,36 +12447,30 @@
       <c r="F466" s="2"/>
     </row>
     <row r="467" spans="1:6">
-      <c r="A467" s="2" t="s">
+      <c r="A467" s="2"/>
+      <c r="B467" s="2"/>
+      <c r="C467" s="2" t="s">
         <v>1571</v>
       </c>
-      <c r="B467" s="2" t="s">
+      <c r="D467" s="2" t="s">
         <v>1572</v>
       </c>
-      <c r="C467" s="2" t="s">
+      <c r="E467" s="2" t="s">
         <v>1573</v>
       </c>
-      <c r="D467" s="2" t="s">
-        <v>1571</v>
-      </c>
-      <c r="E467" s="2" t="s">
-        <v>1574</v>
-      </c>
-      <c r="F467" s="2">
-        <v>8</v>
-      </c>
+      <c r="F467" s="2"/>
     </row>
     <row r="468" spans="1:6">
       <c r="A468" s="2"/>
       <c r="B468" s="2"/>
       <c r="C468" s="2" t="s">
+        <v>1574</v>
+      </c>
+      <c r="D468" s="2" t="s">
         <v>1575</v>
       </c>
-      <c r="D468" s="2" t="s">
+      <c r="E468" s="2" t="s">
         <v>1576</v>
-      </c>
-      <c r="E468" s="2" t="s">
-        <v>1577</v>
       </c>
       <c r="F468" s="2"/>
     </row>
@@ -12283,29 +12478,35 @@
       <c r="A469" s="2"/>
       <c r="B469" s="2"/>
       <c r="C469" s="2" t="s">
+        <v>1577</v>
+      </c>
+      <c r="D469" s="2" t="s">
         <v>1578</v>
       </c>
-      <c r="D469" s="2" t="s">
+      <c r="E469" s="2" t="s">
         <v>1579</v>
       </c>
-      <c r="E469" s="2" t="s">
+      <c r="F469" s="2"/>
+    </row>
+    <row r="470" spans="1:6">
+      <c r="A470" s="2" t="s">
         <v>1580</v>
       </c>
-      <c r="F469" s="2"/>
-    </row>
-    <row r="470" spans="1:6">
-      <c r="A470" s="2"/>
-      <c r="B470" s="2"/>
+      <c r="B470" s="2" t="s">
+        <v>1581</v>
+      </c>
       <c r="C470" s="2" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="D470" s="2" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
       <c r="E470" s="2" t="s">
         <v>1583</v>
       </c>
-      <c r="F470" s="2"/>
+      <c r="F470" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="471" spans="1:6">
       <c r="A471" s="2"/>
@@ -12322,104 +12523,98 @@
       <c r="F471" s="2"/>
     </row>
     <row r="472" spans="1:6">
-      <c r="A472" s="2" t="s">
+      <c r="A472" s="2"/>
+      <c r="B472" s="2"/>
+      <c r="C472" s="2" t="s">
         <v>1587</v>
       </c>
-      <c r="B472" s="2" t="s">
+      <c r="D472" s="2" t="s">
         <v>1588</v>
       </c>
-      <c r="C472" s="2" t="s">
-        <v>1308</v>
-      </c>
-      <c r="D472" s="2" t="s">
-        <v>1309</v>
-      </c>
       <c r="E472" s="2" t="s">
-        <v>1310</v>
-      </c>
-      <c r="F472" s="2">
-        <v>7</v>
-      </c>
+        <v>1589</v>
+      </c>
+      <c r="F472" s="2"/>
     </row>
     <row r="473" spans="1:6">
-      <c r="A473" s="2" t="s">
-        <v>1589</v>
-      </c>
-      <c r="B473" s="2" t="s">
+      <c r="A473" s="2"/>
+      <c r="B473" s="2"/>
+      <c r="C473" s="2" t="s">
         <v>1590</v>
       </c>
-      <c r="C473" s="2" t="s">
-        <v>793</v>
-      </c>
       <c r="D473" s="2" t="s">
-        <v>794</v>
+        <v>1591</v>
       </c>
       <c r="E473" s="2" t="s">
-        <v>795</v>
-      </c>
-      <c r="F473" s="2">
-        <v>16</v>
-      </c>
+        <v>1592</v>
+      </c>
+      <c r="F473" s="2"/>
     </row>
     <row r="474" spans="1:6">
       <c r="A474" s="2"/>
       <c r="B474" s="2"/>
       <c r="C474" s="2" t="s">
-        <v>1591</v>
+        <v>1593</v>
       </c>
       <c r="D474" s="2" t="s">
-        <v>1592</v>
+        <v>1594</v>
       </c>
       <c r="E474" s="2" t="s">
-        <v>1593</v>
+        <v>1595</v>
       </c>
       <c r="F474" s="2"/>
     </row>
     <row r="475" spans="1:6">
-      <c r="A475" s="2"/>
-      <c r="B475" s="2"/>
+      <c r="A475" s="2" t="s">
+        <v>1596</v>
+      </c>
+      <c r="B475" s="2" t="s">
+        <v>1597</v>
+      </c>
       <c r="C475" s="2" t="s">
-        <v>966</v>
+        <v>1317</v>
       </c>
       <c r="D475" s="2" t="s">
-        <v>967</v>
+        <v>1318</v>
       </c>
       <c r="E475" s="2" t="s">
-        <v>1594</v>
-      </c>
-      <c r="F475" s="2"/>
+        <v>1319</v>
+      </c>
+      <c r="F475" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="476" spans="1:6">
       <c r="A476" s="2" t="s">
-        <v>1595</v>
+        <v>1598</v>
       </c>
       <c r="B476" s="2" t="s">
-        <v>1596</v>
+        <v>1599</v>
       </c>
       <c r="C476" s="2" t="s">
-        <v>1597</v>
+        <v>793</v>
       </c>
       <c r="D476" s="2" t="s">
-        <v>1595</v>
+        <v>794</v>
       </c>
       <c r="E476" s="2" t="s">
-        <v>1598</v>
+        <v>795</v>
       </c>
       <c r="F476" s="2">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="477" spans="1:6">
       <c r="A477" s="2"/>
       <c r="B477" s="2"/>
       <c r="C477" s="2" t="s">
-        <v>1599</v>
+        <v>1600</v>
       </c>
       <c r="D477" s="2" t="s">
-        <v>1600</v>
+        <v>1601</v>
       </c>
       <c r="E477" s="2" t="s">
-        <v>1601</v>
+        <v>1602</v>
       </c>
       <c r="F477" s="2"/>
     </row>
@@ -12427,29 +12622,35 @@
       <c r="A478" s="2"/>
       <c r="B478" s="2"/>
       <c r="C478" s="2" t="s">
-        <v>1602</v>
+        <v>966</v>
       </c>
       <c r="D478" s="2" t="s">
+        <v>967</v>
+      </c>
+      <c r="E478" s="2" t="s">
         <v>1603</v>
       </c>
-      <c r="E478" s="2" t="s">
+      <c r="F478" s="2"/>
+    </row>
+    <row r="479" spans="1:6">
+      <c r="A479" s="2" t="s">
         <v>1604</v>
       </c>
-      <c r="F478" s="2"/>
-    </row>
-    <row r="479" spans="1:6">
-      <c r="A479" s="2"/>
-      <c r="B479" s="2"/>
+      <c r="B479" s="2" t="s">
+        <v>1605</v>
+      </c>
       <c r="C479" s="2" t="s">
-        <v>1605</v>
+        <v>1606</v>
       </c>
       <c r="D479" s="2" t="s">
-        <v>1606</v>
+        <v>1604</v>
       </c>
       <c r="E479" s="2" t="s">
         <v>1607</v>
       </c>
-      <c r="F479" s="2"/>
+      <c r="F479" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="480" spans="1:6">
       <c r="A480" s="2"/>
@@ -12480,114 +12681,102 @@
       <c r="F481" s="2"/>
     </row>
     <row r="482" spans="1:6">
-      <c r="A482" s="2" t="s">
+      <c r="A482" s="2"/>
+      <c r="B482" s="2"/>
+      <c r="C482" s="2" t="s">
         <v>1614</v>
       </c>
-      <c r="B482" s="2" t="s">
+      <c r="D482" s="2" t="s">
         <v>1615</v>
       </c>
-      <c r="C482" s="2" t="s">
+      <c r="E482" s="2" t="s">
         <v>1616</v>
       </c>
-      <c r="D482" s="2" t="s">
+      <c r="F482" s="2"/>
+    </row>
+    <row r="483" spans="1:6">
+      <c r="A483" s="2"/>
+      <c r="B483" s="2"/>
+      <c r="C483" s="2" t="s">
         <v>1617</v>
       </c>
-      <c r="E482" s="2" t="s">
+      <c r="D483" s="2" t="s">
         <v>1618</v>
       </c>
-      <c r="F482" s="2">
+      <c r="E483" s="2" t="s">
+        <v>1619</v>
+      </c>
+      <c r="F483" s="2"/>
+    </row>
+    <row r="484" spans="1:6">
+      <c r="A484" s="2"/>
+      <c r="B484" s="2"/>
+      <c r="C484" s="2" t="s">
+        <v>1620</v>
+      </c>
+      <c r="D484" s="2" t="s">
+        <v>1621</v>
+      </c>
+      <c r="E484" s="2" t="s">
+        <v>1622</v>
+      </c>
+      <c r="F484" s="2"/>
+    </row>
+    <row r="485" spans="1:6">
+      <c r="A485" s="2" t="s">
+        <v>1623</v>
+      </c>
+      <c r="B485" s="2" t="s">
+        <v>1624</v>
+      </c>
+      <c r="C485" s="2" t="s">
+        <v>1625</v>
+      </c>
+      <c r="D485" s="2" t="s">
+        <v>1626</v>
+      </c>
+      <c r="E485" s="2" t="s">
+        <v>1627</v>
+      </c>
+      <c r="F485" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="483" spans="1:6">
-      <c r="A483" s="2" t="s">
-        <v>1619</v>
-      </c>
-      <c r="B483" s="2" t="s">
-        <v>1620</v>
-      </c>
-      <c r="C483" s="2" t="s">
-        <v>1621</v>
-      </c>
-      <c r="D483" s="2" t="s">
-        <v>1622</v>
-      </c>
-      <c r="E483" s="2" t="s">
-        <v>1623</v>
-      </c>
-      <c r="F483" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="484" spans="1:6">
-      <c r="A484" s="2" t="s">
-        <v>1624</v>
-      </c>
-      <c r="B484" s="2" t="s">
-        <v>1625</v>
-      </c>
-      <c r="C484" s="2" t="s">
-        <v>1626</v>
-      </c>
-      <c r="D484" s="2" t="s">
-        <v>1627</v>
-      </c>
-      <c r="E484" s="2" t="s">
-        <v>1628</v>
-      </c>
-      <c r="F484" s="2">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="485" spans="1:6">
-      <c r="A485" s="2"/>
-      <c r="B485" s="2"/>
-      <c r="C485" s="2" t="s">
-        <v>1629</v>
-      </c>
-      <c r="D485" s="2" t="s">
-        <v>1630</v>
-      </c>
-      <c r="E485" s="2" t="s">
-        <v>1631</v>
-      </c>
-      <c r="F485" s="2"/>
     </row>
     <row r="486" spans="1:6">
       <c r="A486" s="2" t="s">
+        <v>1628</v>
+      </c>
+      <c r="B486" s="2" t="s">
+        <v>1629</v>
+      </c>
+      <c r="C486" s="2" t="s">
+        <v>1630</v>
+      </c>
+      <c r="D486" s="2" t="s">
+        <v>1631</v>
+      </c>
+      <c r="E486" s="2" t="s">
         <v>1632</v>
       </c>
-      <c r="B486" s="2" t="s">
-        <v>1413</v>
-      </c>
-      <c r="C486" s="2" t="s">
-        <v>1633</v>
-      </c>
-      <c r="D486" s="2" t="s">
-        <v>1634</v>
-      </c>
-      <c r="E486" s="2" t="s">
-        <v>1635</v>
-      </c>
       <c r="F486" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="487" spans="1:6">
       <c r="A487" s="2" t="s">
+        <v>1633</v>
+      </c>
+      <c r="B487" s="2" t="s">
+        <v>1634</v>
+      </c>
+      <c r="C487" s="2" t="s">
+        <v>1635</v>
+      </c>
+      <c r="D487" s="2" t="s">
         <v>1636</v>
       </c>
-      <c r="B487" s="2" t="s">
+      <c r="E487" s="2" t="s">
         <v>1637</v>
-      </c>
-      <c r="C487" s="2" t="s">
-        <v>1638</v>
-      </c>
-      <c r="D487" s="2" t="s">
-        <v>1639</v>
-      </c>
-      <c r="E487" s="2" t="s">
-        <v>1640</v>
       </c>
       <c r="F487" s="2">
         <v>18</v>
@@ -12597,18 +12786,298 @@
       <c r="A488" s="2"/>
       <c r="B488" s="2"/>
       <c r="C488" s="2" t="s">
+        <v>1638</v>
+      </c>
+      <c r="D488" s="2" t="s">
+        <v>1639</v>
+      </c>
+      <c r="E488" s="2" t="s">
+        <v>1640</v>
+      </c>
+      <c r="F488" s="2"/>
+    </row>
+    <row r="489" spans="1:6">
+      <c r="A489" s="2" t="s">
         <v>1641</v>
       </c>
-      <c r="D488" s="2" t="s">
+      <c r="B489" s="2" t="s">
+        <v>1422</v>
+      </c>
+      <c r="C489" s="2" t="s">
         <v>1642</v>
       </c>
-      <c r="E488" s="2" t="s">
+      <c r="D489" s="2" t="s">
         <v>1643</v>
       </c>
-      <c r="F488" s="2"/>
+      <c r="E489" s="2" t="s">
+        <v>1644</v>
+      </c>
+      <c r="F489" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="490" spans="1:6">
+      <c r="A490" s="2" t="s">
+        <v>1645</v>
+      </c>
+      <c r="B490" s="2" t="s">
+        <v>1646</v>
+      </c>
+      <c r="C490" s="2" t="s">
+        <v>1647</v>
+      </c>
+      <c r="D490" s="2" t="s">
+        <v>1648</v>
+      </c>
+      <c r="E490" s="2" t="s">
+        <v>1649</v>
+      </c>
+      <c r="F490" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="491" spans="1:6">
+      <c r="A491" s="2"/>
+      <c r="B491" s="2"/>
+      <c r="C491" s="2" t="s">
+        <v>1650</v>
+      </c>
+      <c r="D491" s="2" t="s">
+        <v>1651</v>
+      </c>
+      <c r="E491" s="2" t="s">
+        <v>1652</v>
+      </c>
+      <c r="F491" s="2"/>
+    </row>
+    <row r="492" spans="1:6">
+      <c r="A492" s="1" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B492" s="1" t="s">
+        <v>1654</v>
+      </c>
+      <c r="C492" s="1" t="s">
+        <v>1655</v>
+      </c>
+      <c r="D492" s="1" t="s">
+        <v>1656</v>
+      </c>
+      <c r="E492" s="1" t="s">
+        <v>1657</v>
+      </c>
+      <c r="F492" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="493" spans="1:6">
+      <c r="C493" s="1" t="s">
+        <v>1658</v>
+      </c>
+      <c r="D493" s="1" t="s">
+        <v>1659</v>
+      </c>
+      <c r="E493" s="1" t="s">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="494" spans="1:6">
+      <c r="A494" s="1" t="s">
+        <v>1661</v>
+      </c>
+      <c r="B494" s="1" t="s">
+        <v>1662</v>
+      </c>
+      <c r="C494" s="1" t="s">
+        <v>1663</v>
+      </c>
+      <c r="D494" s="1" t="s">
+        <v>1661</v>
+      </c>
+      <c r="E494" s="1" t="s">
+        <v>1664</v>
+      </c>
+      <c r="F494" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="495" spans="1:6">
+      <c r="A495" s="1" t="s">
+        <v>1665</v>
+      </c>
+      <c r="B495" s="1" t="s">
+        <v>1666</v>
+      </c>
+      <c r="C495" s="1" t="s">
+        <v>1667</v>
+      </c>
+      <c r="D495" s="1" t="s">
+        <v>1665</v>
+      </c>
+      <c r="E495" s="1" t="s">
+        <v>1668</v>
+      </c>
+      <c r="F495" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="496" spans="1:6">
+      <c r="C496" s="1" t="s">
+        <v>1669</v>
+      </c>
+      <c r="D496" s="1" t="s">
+        <v>1670</v>
+      </c>
+      <c r="E496" s="1" t="s">
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="497" spans="1:6">
+      <c r="C497" s="1" t="s">
+        <v>1672</v>
+      </c>
+      <c r="D497" s="1" t="s">
+        <v>1673</v>
+      </c>
+      <c r="E497" s="1" t="s">
+        <v>1674</v>
+      </c>
+    </row>
+    <row r="498" spans="1:6">
+      <c r="C498" s="1" t="s">
+        <v>1675</v>
+      </c>
+      <c r="D498" s="1" t="s">
+        <v>1676</v>
+      </c>
+      <c r="E498" s="1" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="499" spans="1:6">
+      <c r="A499" s="1" t="s">
+        <v>1678</v>
+      </c>
+      <c r="B499" s="1" t="s">
+        <v>1679</v>
+      </c>
+      <c r="C499" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D499" s="1" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E499" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F499" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="500" spans="1:6">
+      <c r="C500" s="1" t="s">
+        <v>1680</v>
+      </c>
+      <c r="D500" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E500" s="1" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="501" spans="1:6">
+      <c r="A501" s="1" t="s">
+        <v>1683</v>
+      </c>
+      <c r="B501" s="1" t="s">
+        <v>1684</v>
+      </c>
+      <c r="C501" s="1" t="s">
+        <v>1685</v>
+      </c>
+      <c r="D501" s="1" t="s">
+        <v>1683</v>
+      </c>
+      <c r="E501" s="1" t="s">
+        <v>1686</v>
+      </c>
+      <c r="F501" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="502" spans="1:6">
+      <c r="A502" s="1" t="s">
+        <v>1687</v>
+      </c>
+      <c r="B502" s="1" t="s">
+        <v>1688</v>
+      </c>
+      <c r="C502" s="1" t="s">
+        <v>1689</v>
+      </c>
+      <c r="D502" s="1" t="s">
+        <v>1690</v>
+      </c>
+      <c r="E502" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="F502" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="503" spans="1:6">
+      <c r="A503" s="1" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B503" s="1" t="s">
+        <v>1692</v>
+      </c>
+      <c r="C503" s="1" t="s">
+        <v>1693</v>
+      </c>
+      <c r="D503" s="1" t="s">
+        <v>1691</v>
+      </c>
+      <c r="E503" s="1" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F503" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="504" spans="1:6">
+      <c r="C504" s="1" t="s">
+        <v>1695</v>
+      </c>
+      <c r="D504" s="1" t="s">
+        <v>1696</v>
+      </c>
+      <c r="E504" s="1" t="s">
+        <v>1697</v>
+      </c>
+    </row>
+    <row r="505" spans="1:6">
+      <c r="A505" s="1" t="s">
+        <v>1698</v>
+      </c>
+      <c r="B505" s="1" t="s">
+        <v>1699</v>
+      </c>
+      <c r="C505" s="1" t="s">
+        <v>1700</v>
+      </c>
+      <c r="D505" s="1" t="s">
+        <v>1698</v>
+      </c>
+      <c r="E505" s="1" t="s">
+        <v>1701</v>
+      </c>
+      <c r="F505" s="1">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E421" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E424" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -12619,7 +13088,7 @@
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -12631,19 +13100,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -12651,23 +13120,23 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="18.75">
-      <c r="A2" s="1" t="s">
-        <v>1644</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1645</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1646</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>1647</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>1648</v>
-      </c>
-      <c r="F2" s="1">
-        <v>4</v>
+      <c r="A2" s="2" t="s">
+        <v>1702</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1703</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1704</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1705</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>1706</v>
+      </c>
+      <c r="F2" s="2">
+        <v>12</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -12676,18 +13145,18 @@
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:18" ht="18.75">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
-        <v>1649</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>1650</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>1651</v>
-      </c>
-      <c r="F3" s="1"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>1707</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>1708</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>1709</v>
+      </c>
+      <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -12695,24 +13164,18 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:18" ht="18.75">
-      <c r="A4" s="1" t="s">
-        <v>1652</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>1653</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>1654</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>1652</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>1655</v>
-      </c>
-      <c r="F4" s="1">
-        <v>7</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>1710</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>1708</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>1711</v>
+      </c>
+      <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -12720,24 +13183,18 @@
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:18" ht="18.75">
-      <c r="A5" s="1" t="s">
-        <v>1656</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>1657</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>1658</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>1656</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>1659</v>
-      </c>
-      <c r="F5" s="1">
-        <v>9</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>1712</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -12745,18 +13202,24 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:18" ht="18.75">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1" t="s">
-        <v>1660</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>1661</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>1662</v>
-      </c>
-      <c r="F6" s="1"/>
+      <c r="A6" s="2" t="s">
+        <v>1715</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1716</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>1717</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>1718</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F6" s="2">
+        <v>11</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -12764,18 +13227,18 @@
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:18" ht="18.75">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1" t="s">
-        <v>1663</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>1664</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>1665</v>
-      </c>
-      <c r="F7" s="1"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>1720</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>1721</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>1722</v>
+      </c>
+      <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -12783,18 +13246,18 @@
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:18" ht="18.75">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1" t="s">
-        <v>1666</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>1667</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>1668</v>
-      </c>
-      <c r="F8" s="1"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>1723</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>1724</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>1725</v>
+      </c>
+      <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -12802,23 +13265,23 @@
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:18" ht="18.75">
-      <c r="A9" s="1" t="s">
-        <v>1669</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>1670</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>1002</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>1003</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>1004</v>
-      </c>
-      <c r="F9" s="1">
-        <v>6</v>
+      <c r="A9" s="2" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1727</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>1728</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>1729</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>1730</v>
+      </c>
+      <c r="F9" s="2">
+        <v>9</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -12827,18 +13290,18 @@
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:18" ht="18.75">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
-        <v>1671</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>1672</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>1673</v>
-      </c>
-      <c r="F10" s="1"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>1731</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>1732</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>1733</v>
+      </c>
+      <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -12853,24 +13316,18 @@
       <c r="R10" s="2"/>
     </row>
     <row r="11" spans="1:18" ht="18.75">
-      <c r="A11" s="1" t="s">
-        <v>1674</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>1675</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>1676</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>1674</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>1677</v>
-      </c>
-      <c r="F11" s="1">
-        <v>6</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>1734</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>1735</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>1736</v>
+      </c>
+      <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -12885,24 +13342,18 @@
       <c r="R11" s="2"/>
     </row>
     <row r="12" spans="1:18" ht="18.75">
-      <c r="A12" s="1" t="s">
-        <v>1678</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>1679</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>1680</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>1681</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="F12" s="1">
-        <v>3</v>
-      </c>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>1737</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>1738</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>1739</v>
+      </c>
+      <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -12917,23 +13368,23 @@
       <c r="R12" s="2"/>
     </row>
     <row r="13" spans="1:18" ht="18.75">
-      <c r="A13" s="1" t="s">
-        <v>1682</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>1683</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>1684</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>1682</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>1685</v>
-      </c>
-      <c r="F13" s="1">
-        <v>5</v>
+      <c r="A13" s="2" t="s">
+        <v>1740</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>1741</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>1742</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>1743</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F13" s="2">
+        <v>7</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -12949,18 +13400,18 @@
       <c r="R13" s="2"/>
     </row>
     <row r="14" spans="1:18" ht="18.75">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1" t="s">
-        <v>1686</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>1687</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>1688</v>
-      </c>
-      <c r="F14" s="1"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>1587</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>1588</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>1589</v>
+      </c>
+      <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -12975,23 +13426,23 @@
       <c r="R14" s="2"/>
     </row>
     <row r="15" spans="1:18" ht="18.75">
-      <c r="A15" s="1" t="s">
-        <v>1689</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>1690</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>1691</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>1689</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>1692</v>
-      </c>
-      <c r="F15" s="1">
-        <v>11</v>
+      <c r="A15" s="2" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>1559</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>1560</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>1746</v>
+      </c>
+      <c r="F15" s="2">
+        <v>9</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -13009,9 +13460,15 @@
     <row r="16" spans="1:18" ht="18.75">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>1747</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>1748</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>1749</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -13029,9 +13486,15 @@
     <row r="17" spans="1:18" ht="18.75">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>1750</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>1751</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>1752</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -13047,12 +13510,24 @@
       <c r="R17" s="2"/>
     </row>
     <row r="18" spans="1:18" ht="18.75">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="A18" s="2" t="s">
+        <v>1753</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>1754</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>1755</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>1756</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>1757</v>
+      </c>
+      <c r="F18" s="2">
+        <v>10</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -13069,9 +13544,15 @@
     <row r="19" spans="1:18" ht="18.75">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>1758</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>1756</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>1759</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -13089,9 +13570,15 @@
     <row r="20" spans="1:18" ht="18.75">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>1760</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>1761</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>1762</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>

</xml_diff>

<commit_message>
update load file excel
</commit_message>
<xml_diff>
--- a/kanji.xlsx
+++ b/kanji.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21728"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A372AEB0-0627-41E5-8043-527B9FDF0F60}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A11EF48E-3C19-4D6A-B1BC-BADB9BD7F834}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28695" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="28695" windowHeight="12525" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2186" uniqueCount="1925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2217" uniqueCount="1928">
   <si>
     <t>Chữ hán</t>
   </si>
@@ -5803,6 +5803,15 @@
   </si>
   <si>
     <t>xa</t>
+  </si>
+  <si>
+    <t>とおく</t>
+  </si>
+  <si>
+    <t>遠く</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> xa (adv)</t>
   </si>
 </sst>
 </file>
@@ -6196,8 +6205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H573"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A558" workbookViewId="0">
-      <selection activeCell="A566" sqref="A566"/>
+    <sheetView topLeftCell="A511" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
@@ -14603,8 +14612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14820,9 +14829,15 @@
     <row r="10" spans="1:18" ht="18.75">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>1925</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>1926</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1927</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -14831,12 +14846,24 @@
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:18" ht="18.75">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="1">
+        <v>4</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -14853,9 +14880,15 @@
     <row r="12" spans="1:18" ht="18.75">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -14873,9 +14906,15 @@
     <row r="13" spans="1:18" ht="18.75">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -14891,12 +14930,24 @@
       <c r="R13" s="2"/>
     </row>
     <row r="14" spans="1:18" ht="18.75">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="1">
+        <v>4</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -14913,9 +14964,15 @@
     <row r="15" spans="1:18" ht="18.75">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -14933,9 +14990,15 @@
     <row r="16" spans="1:18" ht="18.75">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="F16" s="1"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -14953,9 +15016,15 @@
     <row r="17" spans="1:18" ht="18.75">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="F17" s="1"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -14973,9 +15042,15 @@
     <row r="18" spans="1:18" ht="18.75">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>

</xml_diff>

<commit_message>
update kanji and model
</commit_message>
<xml_diff>
--- a/kanji.xlsx
+++ b/kanji.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21823"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21903"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41753FF6-FD88-4AD2-B779-C1F3E02C7C4A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B21A5D3-74CD-4603-8BC2-0435DD48ED9B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="28695" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2583" uniqueCount="2271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2643" uniqueCount="2325">
   <si>
     <t>Chữ hán</t>
   </si>
@@ -6832,6 +6832,168 @@
   </si>
   <si>
     <t>tế bào</t>
+  </si>
+  <si>
+    <t>池</t>
+  </si>
+  <si>
+    <t>いけ</t>
+  </si>
+  <si>
+    <t>ao</t>
+  </si>
+  <si>
+    <t>でんち</t>
+  </si>
+  <si>
+    <t>電池</t>
+  </si>
+  <si>
+    <t>pin</t>
+  </si>
+  <si>
+    <t>公</t>
+  </si>
+  <si>
+    <t>công</t>
+  </si>
+  <si>
+    <t>こうえん</t>
+  </si>
+  <si>
+    <t>公園</t>
+  </si>
+  <si>
+    <t>công viên</t>
+  </si>
+  <si>
+    <t>おおやけ</t>
+  </si>
+  <si>
+    <t>công cộng</t>
+  </si>
+  <si>
+    <t>園</t>
+  </si>
+  <si>
+    <t>viên</t>
+  </si>
+  <si>
+    <t>どうぶつえん</t>
+  </si>
+  <si>
+    <t>動物園</t>
+  </si>
+  <si>
+    <t>sở thú</t>
+  </si>
+  <si>
+    <t>ようちえん</t>
+  </si>
+  <si>
+    <t>幼稚園</t>
+  </si>
+  <si>
+    <t>nhà trẻ</t>
+  </si>
+  <si>
+    <t>洋</t>
+  </si>
+  <si>
+    <t>dương</t>
+  </si>
+  <si>
+    <t>ようふく</t>
+  </si>
+  <si>
+    <t>洋服</t>
+  </si>
+  <si>
+    <t>quần áo tây</t>
+  </si>
+  <si>
+    <t>せいようかする</t>
+  </si>
+  <si>
+    <t>西洋化する</t>
+  </si>
+  <si>
+    <t>tây hóa</t>
+  </si>
+  <si>
+    <t>ようしょく</t>
+  </si>
+  <si>
+    <t>洋食</t>
+  </si>
+  <si>
+    <t>đồ ăn tây</t>
+  </si>
+  <si>
+    <t>かいよう</t>
+  </si>
+  <si>
+    <t>海洋</t>
+  </si>
+  <si>
+    <t>hải dương</t>
+  </si>
+  <si>
+    <t>辺</t>
+  </si>
+  <si>
+    <t>biên</t>
+  </si>
+  <si>
+    <t>～へん</t>
+  </si>
+  <si>
+    <t>～辺</t>
+  </si>
+  <si>
+    <t>khu vực ~</t>
+  </si>
+  <si>
+    <t>あたり</t>
+  </si>
+  <si>
+    <t>辺り</t>
+  </si>
+  <si>
+    <t xml:space="preserve">khu vực </t>
+  </si>
+  <si>
+    <t>交</t>
+  </si>
+  <si>
+    <t>giao</t>
+  </si>
+  <si>
+    <t>こうつう</t>
+  </si>
+  <si>
+    <t>交通</t>
+  </si>
+  <si>
+    <t>giao thông</t>
+  </si>
+  <si>
+    <t>こうさてん</t>
+  </si>
+  <si>
+    <t>交差点</t>
+  </si>
+  <si>
+    <t>ngã tư</t>
+  </si>
+  <si>
+    <t>こうばん</t>
+  </si>
+  <si>
+    <t>交番</t>
+  </si>
+  <si>
+    <t>đồn cảnh sát</t>
   </si>
   <si>
     <t>とおく</t>
@@ -7238,10 +7400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H681"/>
+  <dimension ref="A1:H697"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A666" workbookViewId="0">
-      <selection activeCell="A679" sqref="A679"/>
+    <sheetView tabSelected="1" topLeftCell="A687" workbookViewId="0">
+      <selection activeCell="F696" sqref="F696"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
@@ -7307,11 +7469,11 @@
       </c>
       <c r="G2" s="1">
         <f>COUNTA(A2:A100100)</f>
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="H2" s="1">
         <f>COUNTA(C2:C10100)</f>
-        <v>680</v>
+        <v>696</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -17050,6 +17212,236 @@
       </c>
       <c r="E681" s="1" t="s">
         <v>2267</v>
+      </c>
+    </row>
+    <row r="682" spans="1:6">
+      <c r="A682" s="1" t="s">
+        <v>2268</v>
+      </c>
+      <c r="B682" s="1" t="s">
+        <v>1829</v>
+      </c>
+      <c r="C682" s="1" t="s">
+        <v>2269</v>
+      </c>
+      <c r="D682" s="1" t="s">
+        <v>2268</v>
+      </c>
+      <c r="E682" s="1" t="s">
+        <v>2270</v>
+      </c>
+      <c r="F682" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="683" spans="1:6">
+      <c r="C683" s="1" t="s">
+        <v>2271</v>
+      </c>
+      <c r="D683" s="1" t="s">
+        <v>2272</v>
+      </c>
+      <c r="E683" s="1" t="s">
+        <v>2273</v>
+      </c>
+    </row>
+    <row r="684" spans="1:6">
+      <c r="A684" s="1" t="s">
+        <v>2274</v>
+      </c>
+      <c r="B684" s="1" t="s">
+        <v>2275</v>
+      </c>
+      <c r="C684" s="1" t="s">
+        <v>2276</v>
+      </c>
+      <c r="D684" s="1" t="s">
+        <v>2277</v>
+      </c>
+      <c r="E684" s="1" t="s">
+        <v>2278</v>
+      </c>
+      <c r="F684" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="685" spans="1:6">
+      <c r="C685" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="D685" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="E685" s="1" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="686" spans="1:6">
+      <c r="C686" s="1" t="s">
+        <v>2279</v>
+      </c>
+      <c r="D686" s="1" t="s">
+        <v>2274</v>
+      </c>
+      <c r="E686" s="1" t="s">
+        <v>2280</v>
+      </c>
+    </row>
+    <row r="687" spans="1:6">
+      <c r="A687" s="1" t="s">
+        <v>2281</v>
+      </c>
+      <c r="B687" s="1" t="s">
+        <v>2282</v>
+      </c>
+      <c r="C687" s="1" t="s">
+        <v>2283</v>
+      </c>
+      <c r="D687" s="1" t="s">
+        <v>2284</v>
+      </c>
+      <c r="E687" s="1" t="s">
+        <v>2285</v>
+      </c>
+      <c r="F687" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="688" spans="1:6">
+      <c r="C688" s="1" t="s">
+        <v>2286</v>
+      </c>
+      <c r="D688" s="1" t="s">
+        <v>2287</v>
+      </c>
+      <c r="E688" s="1" t="s">
+        <v>2288</v>
+      </c>
+    </row>
+    <row r="689" spans="1:6">
+      <c r="A689" s="1" t="s">
+        <v>2289</v>
+      </c>
+      <c r="B689" s="1" t="s">
+        <v>2290</v>
+      </c>
+      <c r="C689" s="1" t="s">
+        <v>2291</v>
+      </c>
+      <c r="D689" s="1" t="s">
+        <v>2292</v>
+      </c>
+      <c r="E689" s="1" t="s">
+        <v>2293</v>
+      </c>
+      <c r="F689" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="690" spans="1:6">
+      <c r="C690" s="1" t="s">
+        <v>2294</v>
+      </c>
+      <c r="D690" s="1" t="s">
+        <v>2295</v>
+      </c>
+      <c r="E690" s="1" t="s">
+        <v>2296</v>
+      </c>
+    </row>
+    <row r="691" spans="1:6">
+      <c r="C691" s="1" t="s">
+        <v>2297</v>
+      </c>
+      <c r="D691" s="1" t="s">
+        <v>2298</v>
+      </c>
+      <c r="E691" s="1" t="s">
+        <v>2299</v>
+      </c>
+    </row>
+    <row r="692" spans="1:6">
+      <c r="C692" s="1" t="s">
+        <v>2300</v>
+      </c>
+      <c r="D692" s="1" t="s">
+        <v>2301</v>
+      </c>
+      <c r="E692" s="1" t="s">
+        <v>2302</v>
+      </c>
+    </row>
+    <row r="693" spans="1:6">
+      <c r="A693" s="1" t="s">
+        <v>2303</v>
+      </c>
+      <c r="B693" s="1" t="s">
+        <v>2304</v>
+      </c>
+      <c r="C693" s="1" t="s">
+        <v>2305</v>
+      </c>
+      <c r="D693" s="1" t="s">
+        <v>2306</v>
+      </c>
+      <c r="E693" s="1" t="s">
+        <v>2307</v>
+      </c>
+      <c r="F693" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="694" spans="1:6">
+      <c r="C694" s="1" t="s">
+        <v>2308</v>
+      </c>
+      <c r="D694" s="1" t="s">
+        <v>2309</v>
+      </c>
+      <c r="E694" s="1" t="s">
+        <v>2310</v>
+      </c>
+    </row>
+    <row r="695" spans="1:6">
+      <c r="A695" s="1" t="s">
+        <v>2311</v>
+      </c>
+      <c r="B695" s="1" t="s">
+        <v>2312</v>
+      </c>
+      <c r="C695" s="1" t="s">
+        <v>2313</v>
+      </c>
+      <c r="D695" s="1" t="s">
+        <v>2314</v>
+      </c>
+      <c r="E695" s="1" t="s">
+        <v>2315</v>
+      </c>
+      <c r="F695" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="696" spans="1:6">
+      <c r="C696" s="1" t="s">
+        <v>2316</v>
+      </c>
+      <c r="D696" s="1" t="s">
+        <v>2317</v>
+      </c>
+      <c r="E696" s="1" t="s">
+        <v>2318</v>
+      </c>
+    </row>
+    <row r="697" spans="1:6">
+      <c r="C697" s="1" t="s">
+        <v>2319</v>
+      </c>
+      <c r="D697" s="1" t="s">
+        <v>2320</v>
+      </c>
+      <c r="E697" s="1" t="s">
+        <v>2321</v>
       </c>
     </row>
   </sheetData>
@@ -17063,7 +17455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -17281,13 +17673,13 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>2268</v>
+        <v>2322</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>2269</v>
+        <v>2323</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>2270</v>
+        <v>2324</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="2"/>

</xml_diff>

<commit_message>
git add grammar part
</commit_message>
<xml_diff>
--- a/kanji.xlsx
+++ b/kanji.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C66BC884-01D8-4299-9DD5-C9E913E31DF4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28695" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="28695" windowHeight="12525" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$391</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3051" uniqueCount="2756">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3311" uniqueCount="2926">
   <si>
     <t>Chữ hán</t>
   </si>
@@ -8296,17 +8295,766 @@
   </si>
   <si>
     <t>Anh vẽ bản đồ giúp tôi được không ạ</t>
+  </si>
+  <si>
+    <t>Vる/Vている/Vた + ところです</t>
+  </si>
+  <si>
+    <t>Chuẩn bị làm, đang làm, vừa làm(nhấn mạnh thời điểm xảy ra)</t>
+  </si>
+  <si>
+    <t>会議は　今から　始まる　ところです</t>
+  </si>
+  <si>
+    <t>Cuộc họp sẽ bắt đầu bây giờ.</t>
+  </si>
+  <si>
+    <t>今手紙を書いているところなので,後でお茶を飲みます</t>
+  </si>
+  <si>
+    <t>Bây giờ vì tôi đang viết thư nên tôi sẽ uống trà sau</t>
+  </si>
+  <si>
+    <t>たったいま, バスが出たところです</t>
+  </si>
+  <si>
+    <t>Xe bus vừa mới ra</t>
+  </si>
+  <si>
+    <t>Vたばかりです</t>
+  </si>
+  <si>
+    <t>Vừa mới làm gì(nghĩa rộng hơn bao hàm cả ý người nói cho rằng sự việc mới xảy ra)</t>
+  </si>
+  <si>
+    <t>Anh ấy mới tốt nghiệp đại học vào tháng 3</t>
+  </si>
+  <si>
+    <t>先月　会社に　入った　ばかりなので,まだ　よく　わかりません</t>
+  </si>
+  <si>
+    <t>Tôi mới vào công ty tháng trước nên vẫn chưa nắm được hết</t>
+  </si>
+  <si>
+    <t>Vる/Vた/Vない/Aい/Aな/Nの + 場合は</t>
+  </si>
+  <si>
+    <t>Trong trường hợp/khi~</t>
+  </si>
+  <si>
+    <t>カードを　なくした　場合は, すぐ　カード会社に　連絡してください</t>
+  </si>
+  <si>
+    <t>Trong trường hợp đánh mất thẻ thì hãy liên lạc với công ty thẻ ngay</t>
+  </si>
+  <si>
+    <t>地震で　電車が　止まった　場合は，無理に　帰らないで，会社に　泊まって　ください</t>
+  </si>
+  <si>
+    <t>Trong trường hợp tàu điện không hoạt động do động đất thì anh/chị đừng có cố gắng về nhà mà hãy ở lại công ty</t>
+  </si>
+  <si>
+    <t>Vtt/Aい/Aな/Nな＋のに</t>
+  </si>
+  <si>
+    <t>Thế mà, vậy mà</t>
+  </si>
+  <si>
+    <t>約束を　したのに、彼女は　来ませんでした。</t>
+  </si>
+  <si>
+    <t>Tôi đã hẹn với cô ấy, thế mà cô ấy không đến</t>
+  </si>
+  <si>
+    <t>一生懸命　練習して　覚えたのに、途中で　忘れて　しまいました</t>
+  </si>
+  <si>
+    <t>Tôi đã luyện tập kỹ và học thuộc, thế mà đến giữa chừng lại quên mất</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="163"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>ます</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>/A</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="163"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>い</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>/A</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="163"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>な</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>+～すぎます</t>
+    </r>
+  </si>
+  <si>
+    <t>Quá nhiều</t>
+  </si>
+  <si>
+    <t>ゆうべ　お酒を　飲みすぎました</t>
+  </si>
+  <si>
+    <t>笑いすぎて、涙が　出るんです</t>
+  </si>
+  <si>
+    <t>Tối qua tôi uống rượu quá nhiều</t>
+  </si>
+  <si>
+    <t>Tôi cười quá, chảy cả nước mắt</t>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>ます</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>＋やすいです/　にくいです</t>
+    </r>
+  </si>
+  <si>
+    <t>Dễ làm / Khó làm</t>
+  </si>
+  <si>
+    <t>田舎と　町は　どちらが　住みやすいですか</t>
+  </si>
+  <si>
+    <t>この　パソコンは　使いやすいです</t>
+  </si>
+  <si>
+    <t>Cái máy vi tính này dễ sử dụng</t>
+  </si>
+  <si>
+    <t>Nhà quê và thành phố, nơi nào dễ sống hơn</t>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>い</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="163"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>く/A</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>な</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="163"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>に/Nに＋Động từ</t>
+    </r>
+  </si>
+  <si>
+    <t>音を 大きくします</t>
+  </si>
+  <si>
+    <t>Tôi chỉnh âm thanh to hơn</t>
+  </si>
+  <si>
+    <t>もう　夜　遅いですから、静かに　して　いただけませんか</t>
+  </si>
+  <si>
+    <t>Vì đã khuya rồi, làm ơn giữ yên lặng</t>
+  </si>
+  <si>
+    <t>Biến đổi đối tượng(Có thể ko đi với します)</t>
+  </si>
+  <si>
+    <t>～Trông có vẻ</t>
+  </si>
+  <si>
+    <t>上着の　ボタンが　とれそうですよ</t>
+  </si>
+  <si>
+    <t>今にも　雨が　降りそうです</t>
+  </si>
+  <si>
+    <t>この　アルバイト、よさそうですね。給料も　いいし、仕事も　楽そうだし</t>
+  </si>
+  <si>
+    <t>このかばんは　丈夫そうです</t>
+  </si>
+  <si>
+    <t>Cái cúc áo khoác của anh có vẻ sắp tuột rồi đấy</t>
+  </si>
+  <si>
+    <t>Trời có vẻ sắp mưa đến nơi rồi</t>
+  </si>
+  <si>
+    <t>Việc làm thêm này có vẻ tốt nhỉ. Lương cao, công việc lại có vẻ nhàn</t>
+  </si>
+  <si>
+    <t>Chiếc túi xách này có vẻ chắc chắn</t>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>ます</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="163"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>/A</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>い</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="163"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>/A</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>な</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="163"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>＋そうです
+いい -&gt; よさそう
+ない -&gt; なさそう</t>
+    </r>
+  </si>
+  <si>
+    <t>Vて来ます</t>
+  </si>
+  <si>
+    <t>Đi làm V rồi quay về</t>
+  </si>
+  <si>
+    <t>ちょっと　切符を　買って　来ます</t>
+  </si>
+  <si>
+    <t>ちょっと　出かけて　来ます</t>
+  </si>
+  <si>
+    <t>Tôi đi mua vé rồi về</t>
+  </si>
+  <si>
+    <t>Tôi đi ra ngoài rồi về</t>
+  </si>
+  <si>
+    <t>Vる/Nの＋ために</t>
+  </si>
+  <si>
+    <t>Vì ~, Để ~, Cho ~(dạng ý chí, có mục đích rõ ràng)</t>
+  </si>
+  <si>
+    <t>将来　自分の　店を　持つ　ために、貯金して　います。</t>
+  </si>
+  <si>
+    <t>健康の　ために、何か　して　いますか</t>
+  </si>
+  <si>
+    <t>Tôi để dành tiền để mở cửa hàng riêng của mình</t>
+  </si>
+  <si>
+    <t>Hiện giờ anh/chị có làm gì vì sức khỏe không?</t>
+  </si>
+  <si>
+    <t>Vるの/N＋に</t>
+  </si>
+  <si>
+    <t>この　靴は　山を　歩くのに　いいです</t>
+  </si>
+  <si>
+    <t>この　はさみは　花を　切るのに使います</t>
+  </si>
+  <si>
+    <t>この　かばんは　大きくて、旅行に　便利です</t>
+  </si>
+  <si>
+    <t>Đôi giày này thích hợp cho đi bộ trên núi</t>
+  </si>
+  <si>
+    <t>Cái kéo này dùng để cắt hoa</t>
+  </si>
+  <si>
+    <t>Cái túi này to nên rất tiện cho du lịch</t>
+  </si>
+  <si>
+    <t>dùng cho, dùng để ~(sử dụng cho mục đích nào đấy, hoặc dùng để đánh giá là dùng thế này thì tốt/ ko tốt)</t>
+  </si>
+  <si>
+    <t>～によって</t>
+  </si>
+  <si>
+    <t>Biểu đạt các sáng tạo, phát minh bởi ~</t>
+  </si>
+  <si>
+    <t>チキンラーメンは　1958年に　V に　よって　発明されました</t>
+  </si>
+  <si>
+    <t>Ramen vị gà được V sáng chế ra vào năm 1958</t>
+  </si>
+  <si>
+    <t>N1はひとになにかを＋さしあげます／あげます／やります</t>
+  </si>
+  <si>
+    <t>N1 cho, biếu ai cái gì (dùng người trên, cấp trên / người thân ngang hàng / ng ít tuổi, trẻ con, động thực vật)</t>
+  </si>
+  <si>
+    <t>友達に　誕生日のプレゼントを　あげました</t>
+  </si>
+  <si>
+    <t>女性の日に　先生に　花を　さしあげました</t>
+  </si>
+  <si>
+    <t>妹に　おもちゃを　やります</t>
+  </si>
+  <si>
+    <t>Tôi tặng bạn quà sinh nhật</t>
+  </si>
+  <si>
+    <t>Tôi biếu giáo viên hoa vào ngày phụ nữ</t>
+  </si>
+  <si>
+    <t>Tôi cho em gái đồ chơi</t>
+  </si>
+  <si>
+    <t>ひと(から) 　になにかを＋いただきます／もらいます</t>
+  </si>
+  <si>
+    <t>Nhận từ ai đó cái gì(bề trên / ngang hàng hoặc thấp hơn)</t>
+  </si>
+  <si>
+    <t>私は　先生に　漢字の　まちがいを　直して　いただきましたか</t>
+  </si>
+  <si>
+    <t>兄に　すてきなシャツを　もらいました</t>
+  </si>
+  <si>
+    <t>Tôi được thầy giáo sửa cho chỗ sai ở chữ Hán</t>
+  </si>
+  <si>
+    <t>Tôi được anh trai tặng cái áo sơ mi đẹp</t>
+  </si>
+  <si>
+    <t>ひとは（が）なにかを＋くださいます／くれます</t>
+  </si>
+  <si>
+    <t>Ai cho mình cái gì(bề trên / ngang hàng hoặc thấp hơn)</t>
+  </si>
+  <si>
+    <t>部長の　奥さんが　お茶を　教えて　くださいました</t>
+  </si>
+  <si>
+    <t>友達は　本をくれました</t>
+  </si>
+  <si>
+    <t>Vợ của trưởng phòng đã dạy trà đạo cho tôi</t>
+  </si>
+  <si>
+    <t>tôi đã nhận từ bạn quyển sách</t>
+  </si>
+  <si>
+    <t>N1に　N2をV</t>
+  </si>
+  <si>
+    <t>～Làm/để(quà, kỉ niệm)</t>
+  </si>
+  <si>
+    <t>私は　旅行のお土産に　人形を買いました</t>
+  </si>
+  <si>
+    <t>父は入学お祝いに　新しい自転車をくれました</t>
+  </si>
+  <si>
+    <t>Tôi mua con búp bê làm quà lưu niệm cho chuyến du lịch</t>
+  </si>
+  <si>
+    <t>bố tôi mua cho tôi cái xe đạp mới làm quà chúc mừng nhập học</t>
+  </si>
+  <si>
+    <t>Nghi vấn từ＋Vtt／Aい／Aな／N＋か＋V</t>
+  </si>
+  <si>
+    <t>~ Lồng câu nghi vấn vào câu văn(ai/cái gì/khi nào , có biết/hiểu/nhớ không)</t>
+  </si>
+  <si>
+    <t>JL 107 便は　何時に　到着するか、調べて　ください</t>
+  </si>
+  <si>
+    <t>Anh chị kiểm tra xem chuyến bay JL107 đến lúc mấy giờ</t>
+  </si>
+  <si>
+    <t>結婚の　お祝いは　何が　いいか、話しています</t>
+  </si>
+  <si>
+    <t>わたしたちが　初めて　会ったのは　いつか、覚えていますか</t>
+  </si>
+  <si>
+    <t>Chúng tôi đang bàn xem quà mừng đám cưới nên như thế nào</t>
+  </si>
+  <si>
+    <t>Anh/Chị còn nhớ chúng ta gặp nhau lần đầu tiền khi nào không?</t>
+  </si>
+  <si>
+    <t>。。。かどうか。。。</t>
+  </si>
+  <si>
+    <t>Có hay không</t>
+  </si>
+  <si>
+    <t>忘年会に　出席するかどうか、20日までに　返事を　ください</t>
+  </si>
+  <si>
+    <t>Anh/Chị trả lời tôi trước ngày 20 về việc có tham dự được bữa tiệc tất niên hay không</t>
+  </si>
+  <si>
+    <t>その　話は　ほんとうか　どうか、わかりません</t>
+  </si>
+  <si>
+    <t>Tôi không biết chuyện đó có thật hay không</t>
+  </si>
+  <si>
+    <t>まちがいが　ないか　どうか、調べて　ください</t>
+  </si>
+  <si>
+    <t>Anh chị hãy kiểm tra xem có sai sót gì không</t>
+  </si>
+  <si>
+    <t>Vてみます</t>
+  </si>
+  <si>
+    <t>Thử làm việc gì đó</t>
+  </si>
+  <si>
+    <t>もう　一同　考えて　みます</t>
+  </si>
+  <si>
+    <t>この　ズボンを　はいて　みても　いいですか</t>
+  </si>
+  <si>
+    <t>北海道へ　行って　みたいです</t>
+  </si>
+  <si>
+    <t>Tôi sẽ thử nghĩ lại một lần nữa xem</t>
+  </si>
+  <si>
+    <t>Tôi mặc thử cái quần này có được không</t>
+  </si>
+  <si>
+    <t>Tôi muốn đi thử đến hokkaido</t>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>い</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>－＞Aさ</t>
+    </r>
+  </si>
+  <si>
+    <t>Tính từ thành danh từ</t>
+  </si>
+  <si>
+    <t>たかさ</t>
+  </si>
+  <si>
+    <t>ながさ</t>
+  </si>
+  <si>
+    <t>Cân nặng</t>
+  </si>
+  <si>
+    <t>Chiều dài</t>
+  </si>
+  <si>
+    <t>chiều cao</t>
+  </si>
+  <si>
+    <t>Vて/Vない-&gt;Vなくて/Aい-&gt;Aくて/Aな-&gt;Aで/Nで＋～</t>
+  </si>
+  <si>
+    <t>ニュースを　聞いて、びっくりしました</t>
+  </si>
+  <si>
+    <t>家族に　会えなくて、寂しいです</t>
+  </si>
+  <si>
+    <t>土曜日は　都合が　悪くて、行けません</t>
+  </si>
+  <si>
+    <t>話が　複雑で、よく　わかりませんでした</t>
+  </si>
+  <si>
+    <t>Vì, nên ~(Phần kết quả không dùng động từ ý chí hoặc cách nói bao hàm chủ ý như Vたい、Vましょう、Vてください、。。。 Thay vào đó dùng から)
+N thường dùng cho biến cố, sự kiện</t>
+  </si>
+  <si>
+    <t>地震で　ビルが倒れました</t>
+  </si>
+  <si>
+    <t>Tôi ngạc nhiên khi nghe tin</t>
+  </si>
+  <si>
+    <t>Tôi buồn vì không được gặp gia đình</t>
+  </si>
+  <si>
+    <t>Thứ 7 tôi không tiện nên không thể đi được</t>
+  </si>
+  <si>
+    <t>Câu chuyện phức tạp nên tôi không hiểu lắm</t>
+  </si>
+  <si>
+    <t>Tòa nhà đổ do động đất</t>
+  </si>
+  <si>
+    <t>Vtt/Aい/Aな/Nな＋ので、～</t>
+  </si>
+  <si>
+    <t>Vì, nên ~(biểu thị nguyên nhân, lý do khách quan sử dụng khi ng nói muốn khẳng định tính thỏa đáng của lý do mà bản thân đưa ra. から thể hiện lý do chủ quan)</t>
+  </si>
+  <si>
+    <t>日本語が　わからないので。英語で話して　いただけませんか</t>
+  </si>
+  <si>
+    <t>用事が　あるので、お先に　失礼します</t>
+  </si>
+  <si>
+    <t>Vì tôi không hiểu tiếng nhật, nên anh/chị làm ơn nói tiếng anh có được không?</t>
+  </si>
+  <si>
+    <t>Vì có việc nên tôi xin phép về trước</t>
+  </si>
+  <si>
+    <t>Vる／Nの＋途中で</t>
+  </si>
+  <si>
+    <t>Trên đường đi đâu/ làm gì</t>
+  </si>
+  <si>
+    <t>実は　来る　途中で　事故が　あって、バスが遅れてしまったんです</t>
+  </si>
+  <si>
+    <t>マラソンの途中で　気分が悪くなりました</t>
+  </si>
+  <si>
+    <t>Tôi thấy khó chịu khi đang chạy marason</t>
+  </si>
+  <si>
+    <t>Thực ra là trên đường đến đây có một vụ tai nạn nên xe bus bị chậm</t>
+  </si>
+  <si>
+    <t>Vる/Vない/Vた/Vなかった/Aい/Aな＋のはAです／のがAです／のを忘れました／のを知っていますか／のはNです</t>
+  </si>
+  <si>
+    <t>Danh từ hóa động từ, tính từ(の ko sử đụng đc trong mẫu câu 
+Vたことがある／Vることができる／しゅみ(sở thích) còn こと thì được)</t>
+  </si>
+  <si>
+    <t>テニスを　するのは　おもしろいです</t>
+  </si>
+  <si>
+    <t>私は　花を育てるのが　好きです</t>
+  </si>
+  <si>
+    <t>牛乳を　買うのを　忘れました</t>
+  </si>
+  <si>
+    <t>すずきさんが　来月　結婚するのを　知っていますか</t>
+  </si>
+  <si>
+    <t>初めて　会ったのは　いつですか</t>
+  </si>
+  <si>
+    <t>Chơi quần vợt thú vị</t>
+  </si>
+  <si>
+    <t>Tôi thích trồng hoa</t>
+  </si>
+  <si>
+    <t>Tôi quên mua sữa</t>
+  </si>
+  <si>
+    <t>Anh/Chị có biết anh suzuki sẽ cưới vào tháng sau không?</t>
+  </si>
+  <si>
+    <t>Lần đầu tiên anh chị gặp nhau là khi nào</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -8314,7 +9062,7 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Cambria"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="163"/>
       <scheme val="major"/>
@@ -8323,6 +9071,45 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -8345,7 +9132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -8357,9 +9144,13 @@
     </xf>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -8417,7 +9208,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -8449,27 +9240,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -8501,24 +9274,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -8694,26 +9449,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H829"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A784" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E806" sqref="E806"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="2" width="17.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="37.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="17.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.25" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="37.125" style="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="1"/>
-    <col min="8" max="8" width="15.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="21.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19.625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="21.25" style="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -16065,7 +16820,7 @@
       </c>
       <c r="F518" s="2"/>
     </row>
-    <row r="519" spans="1:6" ht="18.75">
+    <row r="519" spans="1:6">
       <c r="A519" s="2"/>
       <c r="B519" s="2"/>
       <c r="C519" s="4" t="s">
@@ -16223,7 +16978,7 @@
       </c>
       <c r="F528" s="2"/>
     </row>
-    <row r="529" spans="1:6" ht="18.75">
+    <row r="529" spans="1:6">
       <c r="A529" s="2"/>
       <c r="B529" s="2"/>
       <c r="C529" s="2" t="s">
@@ -16271,7 +17026,7 @@
       </c>
       <c r="F531" s="2"/>
     </row>
-    <row r="532" spans="1:6" ht="18.75">
+    <row r="532" spans="1:6">
       <c r="A532" s="2"/>
       <c r="B532" s="2"/>
       <c r="C532" s="2" t="s">
@@ -16339,7 +17094,7 @@
       </c>
       <c r="F535" s="2"/>
     </row>
-    <row r="536" spans="1:6" ht="18.75">
+    <row r="536" spans="1:6">
       <c r="A536" s="2"/>
       <c r="B536" s="2"/>
       <c r="C536" s="2" t="s">
@@ -16641,7 +17396,7 @@
       </c>
       <c r="F554" s="2"/>
     </row>
-    <row r="555" spans="1:6" ht="18.75">
+    <row r="555" spans="1:6">
       <c r="A555" s="2"/>
       <c r="B555" s="2"/>
       <c r="C555" s="2" t="s">
@@ -16703,7 +17458,7 @@
       </c>
       <c r="F558" s="2"/>
     </row>
-    <row r="559" spans="1:6" ht="18.75">
+    <row r="559" spans="1:6">
       <c r="A559" s="2"/>
       <c r="B559" s="2"/>
       <c r="C559" s="2" t="s">
@@ -16779,7 +17534,7 @@
       </c>
       <c r="F563" s="2"/>
     </row>
-    <row r="564" spans="1:6" ht="18.75">
+    <row r="564" spans="1:6">
       <c r="A564" s="2"/>
       <c r="B564" s="2"/>
       <c r="C564" s="2" t="s">
@@ -16827,7 +17582,7 @@
       </c>
       <c r="F566" s="2"/>
     </row>
-    <row r="567" spans="1:6" ht="18.75">
+    <row r="567" spans="1:6">
       <c r="A567" s="2"/>
       <c r="B567" s="2"/>
       <c r="C567" s="2" t="s">
@@ -16889,7 +17644,7 @@
       </c>
       <c r="F570" s="2"/>
     </row>
-    <row r="571" spans="1:6" ht="18.75">
+    <row r="571" spans="1:6">
       <c r="A571" s="2"/>
       <c r="B571" s="2"/>
       <c r="C571" s="2" t="s">
@@ -17780,7 +18535,7 @@
         <v>2104</v>
       </c>
     </row>
-    <row r="634" spans="1:6" ht="18.75">
+    <row r="634" spans="1:6">
       <c r="A634" s="2" t="s">
         <v>2105</v>
       </c>
@@ -17800,7 +18555,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="635" spans="1:6" ht="18.75">
+    <row r="635" spans="1:6">
       <c r="A635" s="2"/>
       <c r="B635" s="2"/>
       <c r="C635" s="2" t="s">
@@ -20489,32 +21244,32 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E666" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E666"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:V42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:V66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="38.85546875" customWidth="1"/>
-    <col min="2" max="2" width="44.42578125" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="71.875" customWidth="1"/>
+    <col min="2" max="2" width="44.375" customWidth="1"/>
+    <col min="3" max="3" width="30.75" customWidth="1"/>
     <col min="4" max="4" width="6" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="47.140625" customWidth="1"/>
-    <col min="7" max="7" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="81.125" customWidth="1"/>
+    <col min="7" max="7" width="55.375" customWidth="1"/>
     <col min="8" max="8" width="37" customWidth="1"/>
     <col min="9" max="9" width="25" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="18.75">
@@ -20542,7 +21297,7 @@
       <c r="H1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:22" ht="36">
+    <row r="2" spans="1:22" ht="18.75">
       <c r="A2" s="5" t="s">
         <v>2746</v>
       </c>
@@ -20576,7 +21331,9 @@
     <row r="3" spans="1:22" ht="18.75">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>2748</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
@@ -20597,7 +21354,9 @@
     <row r="4" spans="1:22" ht="18.75">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="6"/>
+      <c r="C4" s="1" t="s">
+        <v>2748</v>
+      </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6" t="s">
@@ -20616,13 +21375,27 @@
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:22" ht="18.75">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="A5" s="3" t="s">
+        <v>2756</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2757</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="D5" s="1">
+        <v>46</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>2749</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>2758</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>2759</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -20635,11 +21408,17 @@
     <row r="6" spans="1:22" ht="18.75">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>2748</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>2760</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>2761</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -20652,11 +21431,17 @@
     <row r="7" spans="1:22" ht="18.75">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>2748</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>2762</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>2763</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -20667,13 +21452,27 @@
       <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:22" ht="18.75">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>2764</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>2765</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="D8" s="1">
+        <v>46</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>2749</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>2750</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>2766</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -20686,6 +21485,15 @@
     <row r="9" spans="1:22" ht="18.75">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>2767</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>2768</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -20696,13 +21504,27 @@
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:22" ht="18.75">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>2769</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>2770</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="D10" s="1">
+        <v>45</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>2749</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>2771</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>2772</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -20711,15 +21533,28 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
     </row>
     <row r="11" spans="1:22" ht="18.75">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>2748</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>2773</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>2774</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -20737,13 +21572,27 @@
       <c r="V11" s="2"/>
     </row>
     <row r="12" spans="1:22" ht="18.75">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>2775</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>2776</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="D12" s="1">
+        <v>45</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>2749</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>2777</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>2778</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -20763,11 +21612,17 @@
     <row r="13" spans="1:22" ht="18.75">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>2748</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>2779</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>2780</v>
+      </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -20785,13 +21640,27 @@
       <c r="V13" s="2"/>
     </row>
     <row r="14" spans="1:22" ht="18.75">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="A14" s="7" t="s">
+        <v>2781</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>2782</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="D14" s="1">
+        <v>44</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>2749</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>2783</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>2785</v>
+      </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -20811,11 +21680,17 @@
     <row r="15" spans="1:22" ht="18.75">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>2748</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="F15" s="1" t="s">
+        <v>2784</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>2786</v>
+      </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -20833,13 +21708,27 @@
       <c r="V15" s="2"/>
     </row>
     <row r="16" spans="1:22" ht="18.75">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>2787</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>2788</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="D16" s="1">
+        <v>44</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>2749</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>2789</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>2792</v>
+      </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -20859,11 +21748,17 @@
     <row r="17" spans="1:22" ht="18.75">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>2748</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>2790</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>2791</v>
+      </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -20881,13 +21776,27 @@
       <c r="V17" s="2"/>
     </row>
     <row r="18" spans="1:22" ht="18.75">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>2793</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>2798</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="D18" s="1">
+        <v>44</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>2749</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>2794</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>2795</v>
+      </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -20907,11 +21816,17 @@
     <row r="19" spans="1:22" ht="18.75">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>2748</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="F19" s="1" t="s">
+        <v>2796</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>2797</v>
+      </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -20928,14 +21843,28 @@
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
     </row>
-    <row r="20" spans="1:22" ht="18.75">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+    <row r="20" spans="1:22" ht="56.25">
+      <c r="A20" s="3" t="s">
+        <v>2808</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>2799</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="D20" s="1">
+        <v>43</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>2749</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>2800</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>2804</v>
+      </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -20955,11 +21884,17 @@
     <row r="21" spans="1:22" ht="18.75">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>2748</v>
+      </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>2801</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>2805</v>
+      </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -20979,11 +21914,17 @@
     <row r="22" spans="1:22" ht="18.75">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="C22" s="1" t="s">
+        <v>2748</v>
+      </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>2802</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>2806</v>
+      </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -21003,11 +21944,17 @@
     <row r="23" spans="1:22" ht="18.75">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="1" t="s">
+        <v>2748</v>
+      </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="F23" s="1" t="s">
+        <v>2803</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>2807</v>
+      </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -21025,13 +21972,27 @@
       <c r="V23" s="2"/>
     </row>
     <row r="24" spans="1:22" ht="18.75">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+      <c r="A24" s="1" t="s">
+        <v>2809</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>2810</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="D24" s="1">
+        <v>43</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>2749</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>2811</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>2813</v>
+      </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -21051,11 +22012,17 @@
     <row r="25" spans="1:22" ht="18.75">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>2748</v>
+      </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
+      <c r="F25" s="1" t="s">
+        <v>2812</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>2814</v>
+      </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -21073,245 +22040,726 @@
       <c r="V25" s="2"/>
     </row>
     <row r="26" spans="1:22" ht="18.75">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>2815</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>2816</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="D26" s="1">
+        <v>42</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>2749</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>2817</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>2819</v>
+      </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
-      <c r="R26" s="2"/>
-      <c r="S26" s="2"/>
-      <c r="T26" s="2"/>
-      <c r="U26" s="2"/>
-      <c r="V26" s="2"/>
     </row>
     <row r="27" spans="1:22" ht="18.75">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="C27" s="1" t="s">
+        <v>2748</v>
+      </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+      <c r="F27" s="1" t="s">
+        <v>2818</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>2820</v>
+      </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="2"/>
-      <c r="R27" s="2"/>
-      <c r="S27" s="2"/>
-      <c r="T27" s="2"/>
-      <c r="U27" s="2"/>
-      <c r="V27" s="2"/>
-    </row>
-    <row r="28" spans="1:22" ht="18">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
+    </row>
+    <row r="28" spans="1:22" ht="18.75">
+      <c r="A28" s="1" t="s">
+        <v>2821</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>2828</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="D28" s="1">
+        <v>42</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>2749</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>2822</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>2825</v>
+      </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:22" ht="18">
+    <row r="29" spans="1:22" ht="18.75">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="C29" s="1" t="s">
+        <v>2748</v>
+      </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
+      <c r="F29" s="1" t="s">
+        <v>2823</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>2826</v>
+      </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:22" ht="18">
+    <row r="30" spans="1:22" ht="18.75">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>2748</v>
+      </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
+      <c r="F30" s="1" t="s">
+        <v>2824</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>2827</v>
+      </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:22" ht="18">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
+    <row r="31" spans="1:22" ht="18.75">
+      <c r="A31" s="1" t="s">
+        <v>2829</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>2830</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="D31" s="1">
+        <v>42</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>2749</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>2831</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>2832</v>
+      </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:22" ht="18">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
+    <row r="32" spans="1:22" ht="18.75">
+      <c r="A32" s="1" t="s">
+        <v>2833</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>2834</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="D32" s="1">
+        <v>41</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>2749</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>2835</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>2838</v>
+      </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10" ht="18">
+    <row r="33" spans="1:10" ht="18.75">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
+      <c r="C33" s="1" t="s">
+        <v>2748</v>
+      </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
+      <c r="F33" s="1" t="s">
+        <v>2836</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>2839</v>
+      </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10" ht="18">
+    <row r="34" spans="1:10" ht="18.75">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
+      <c r="C34" s="1" t="s">
+        <v>2748</v>
+      </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
+      <c r="F34" s="1" t="s">
+        <v>2837</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>2840</v>
+      </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10" ht="18">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
+    <row r="35" spans="1:10" ht="18.75">
+      <c r="A35" s="1" t="s">
+        <v>2841</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>2842</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="D35" s="1">
+        <v>41</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>2749</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>2843</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>2845</v>
+      </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10" ht="18">
+    <row r="36" spans="1:10" ht="18.75">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>2748</v>
+      </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
+      <c r="F36" s="1" t="s">
+        <v>2844</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>2846</v>
+      </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" ht="18">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
+    <row r="37" spans="1:10" ht="18.75">
+      <c r="A37" s="1" t="s">
+        <v>2847</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>2848</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="D37" s="1">
+        <v>41</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>2749</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>2849</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>2851</v>
+      </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10" ht="18">
+    <row r="38" spans="1:10" ht="18.75">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
+      <c r="C38" s="1" t="s">
+        <v>2748</v>
+      </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
+      <c r="F38" s="1" t="s">
+        <v>2850</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>2852</v>
+      </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:10" ht="18">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
+    <row r="39" spans="1:10" ht="18.75">
+      <c r="A39" s="1" t="s">
+        <v>2853</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>2854</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="D39" s="1">
+        <v>41</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>2749</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>2855</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>2857</v>
+      </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="1:10" ht="18">
+    <row r="40" spans="1:10" ht="18.75">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
+      <c r="C40" s="1" t="s">
+        <v>2748</v>
+      </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
+      <c r="F40" s="1" t="s">
+        <v>2856</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>2858</v>
+      </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="1:10" ht="18">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-    </row>
-    <row r="42" spans="1:10" ht="18">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
+    <row r="41" spans="1:10" ht="18.75">
+      <c r="A41" s="1" t="s">
+        <v>2859</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>2860</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="D41" s="1">
+        <v>40</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>2749</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>2861</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>2862</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="18.75">
+      <c r="C42" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>2863</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>2865</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="18.75">
+      <c r="C43" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>2864</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>2866</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="18.75">
+      <c r="A44" t="s">
+        <v>2867</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>2868</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="D44" s="1">
+        <v>40</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>2749</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>2869</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>2870</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="18.75">
+      <c r="C45" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>2871</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>2872</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="18.75">
+      <c r="C46" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>2873</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>2874</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="18.75">
+      <c r="A47" t="s">
+        <v>2875</v>
+      </c>
+      <c r="B47" t="s">
+        <v>2876</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="D47">
+        <v>40</v>
+      </c>
+      <c r="E47" t="s">
+        <v>2749</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>2877</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="18.75">
+      <c r="C48" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>2878</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>2881</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="18.75">
+      <c r="C49" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>2879</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>2882</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="18.75">
+      <c r="A50" t="s">
+        <v>2883</v>
+      </c>
+      <c r="B50" t="s">
+        <v>2884</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="D50">
+        <v>40</v>
+      </c>
+      <c r="E50" t="s">
+        <v>2749</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>1283</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>2887</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="18.75">
+      <c r="C51" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>2885</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>2889</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="18.75">
+      <c r="C52" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>2886</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>2888</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="72.75">
+      <c r="A53" t="s">
+        <v>2890</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>2895</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="D53">
+        <v>39</v>
+      </c>
+      <c r="E53" t="s">
+        <v>2749</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>2891</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>2897</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="18.75">
+      <c r="C54" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>2892</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>2898</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="18.75">
+      <c r="C55" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>2893</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>2899</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="18.75">
+      <c r="C56" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>2894</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="18.75">
+      <c r="C57" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>2896</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>2901</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="18.75">
+      <c r="A58" t="s">
+        <v>2902</v>
+      </c>
+      <c r="B58" t="s">
+        <v>2903</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="D58">
+        <v>39</v>
+      </c>
+      <c r="E58" t="s">
+        <v>2749</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>2904</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>2906</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="18.75">
+      <c r="C59" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>2905</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>2907</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="18.75">
+      <c r="A60" t="s">
+        <v>2908</v>
+      </c>
+      <c r="B60" t="s">
+        <v>2909</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="D60">
+        <v>39</v>
+      </c>
+      <c r="E60" t="s">
+        <v>2749</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>2910</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>2913</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="18.75">
+      <c r="C61" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>2911</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>2912</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="58.5">
+      <c r="A62" t="s">
+        <v>2914</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>2915</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="D62">
+        <v>38</v>
+      </c>
+      <c r="E62" t="s">
+        <v>2749</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>2916</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>2921</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="18.75">
+      <c r="C63" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>2917</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>2922</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="18.75">
+      <c r="C64" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>2918</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>2923</v>
+      </c>
+    </row>
+    <row r="65" spans="3:7" ht="18.75">
+      <c r="C65" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>2919</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>2924</v>
+      </c>
+    </row>
+    <row r="66" spans="3:7" ht="18.75">
+      <c r="C66" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>2920</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>2925</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update kanji remove old word
</commit_message>
<xml_diff>
--- a/kanji.xlsx
+++ b/kanji.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22715"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB785B1D-050D-4871-886B-5D18E855E60C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA1487CB-587D-41CC-BE56-E2E9DE63B30F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="28695" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="1305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1548" uniqueCount="1404">
   <si>
     <t>Chữ hán</t>
   </si>
@@ -3138,6 +3138,303 @@
   </si>
   <si>
     <t>phương hướng</t>
+  </si>
+  <si>
+    <t>打</t>
+  </si>
+  <si>
+    <t>đả</t>
+  </si>
+  <si>
+    <t>うった</t>
+  </si>
+  <si>
+    <t>打った</t>
+  </si>
+  <si>
+    <t>đánh</t>
+  </si>
+  <si>
+    <t>dùng tay đóng đinh</t>
+  </si>
+  <si>
+    <t>だきゅう</t>
+  </si>
+  <si>
+    <t>打球</t>
+  </si>
+  <si>
+    <t>quả bóng đánh</t>
+  </si>
+  <si>
+    <t>きょうだ</t>
+  </si>
+  <si>
+    <t>強打</t>
+  </si>
+  <si>
+    <t>đánh mạnh</t>
+  </si>
+  <si>
+    <t>とうだ</t>
+  </si>
+  <si>
+    <t>投打</t>
+  </si>
+  <si>
+    <t>ném và đánh</t>
+  </si>
+  <si>
+    <t>だてん</t>
+  </si>
+  <si>
+    <t>打点</t>
+  </si>
+  <si>
+    <t>điểm đánh, điểm phát bóng</t>
+  </si>
+  <si>
+    <t>押</t>
+  </si>
+  <si>
+    <t>áp</t>
+  </si>
+  <si>
+    <t>おす</t>
+  </si>
+  <si>
+    <t>押す</t>
+  </si>
+  <si>
+    <t>ấn</t>
+  </si>
+  <si>
+    <t>dùng tay đẩy áo giáp</t>
+  </si>
+  <si>
+    <t>おさえる</t>
+  </si>
+  <si>
+    <t>押さえる</t>
+  </si>
+  <si>
+    <t>giữ chặt</t>
+  </si>
+  <si>
+    <t>おういん</t>
+  </si>
+  <si>
+    <t>押印</t>
+  </si>
+  <si>
+    <t>đóng dấu</t>
+  </si>
+  <si>
+    <t>拾</t>
+  </si>
+  <si>
+    <t>thập</t>
+  </si>
+  <si>
+    <t>ひろう</t>
+  </si>
+  <si>
+    <t>拾う</t>
+  </si>
+  <si>
+    <t>nhặt</t>
+  </si>
+  <si>
+    <t>dùng tay hợp lại(chụm lại) để nhặt đồ</t>
+  </si>
+  <si>
+    <t>しゅうとくぶつ</t>
+  </si>
+  <si>
+    <t>拾得物</t>
+  </si>
+  <si>
+    <t>đồ nhặt được</t>
+  </si>
+  <si>
+    <t>捨</t>
+  </si>
+  <si>
+    <t>xả</t>
+  </si>
+  <si>
+    <t>すてる</t>
+  </si>
+  <si>
+    <t>捨てる</t>
+  </si>
+  <si>
+    <t>vứt</t>
+  </si>
+  <si>
+    <t>đang nhặt đồ 拾 mà xoè 10 ngón tay ra thì phải vứt đồ đi 捨</t>
+  </si>
+  <si>
+    <t>投</t>
+  </si>
+  <si>
+    <t>đầu</t>
+  </si>
+  <si>
+    <t>なげる</t>
+  </si>
+  <si>
+    <t>投げる</t>
+  </si>
+  <si>
+    <t>ném</t>
+  </si>
+  <si>
+    <t>2 tay bê cái bàn đi ném</t>
+  </si>
+  <si>
+    <t>えんとう</t>
+  </si>
+  <si>
+    <t>遠投</t>
+  </si>
+  <si>
+    <t>ném ở khoảng cách xa</t>
+  </si>
+  <si>
+    <t>とうしゅう</t>
+  </si>
+  <si>
+    <t>投手</t>
+  </si>
+  <si>
+    <t>ném liên tục(ko thay ng)</t>
+  </si>
+  <si>
+    <t>とうしょばこ</t>
+  </si>
+  <si>
+    <t>投書箱</t>
+  </si>
+  <si>
+    <t>hòm thư góp ý</t>
+  </si>
+  <si>
+    <t>担ぐ</t>
+  </si>
+  <si>
+    <t>đảm</t>
+  </si>
+  <si>
+    <t>1 tay khiêng cả bầu trời</t>
+  </si>
+  <si>
+    <t>かつがない</t>
+  </si>
+  <si>
+    <t>担が無い</t>
+  </si>
+  <si>
+    <t>đừng mang vác</t>
+  </si>
+  <si>
+    <t>たんとう</t>
+  </si>
+  <si>
+    <t>担当</t>
+  </si>
+  <si>
+    <t>đảm đương</t>
+  </si>
+  <si>
+    <t>ふたん</t>
+  </si>
+  <si>
+    <t>負担</t>
+  </si>
+  <si>
+    <t>Trách nhiệm</t>
+  </si>
+  <si>
+    <t>接</t>
+  </si>
+  <si>
+    <t>tiếp</t>
+  </si>
+  <si>
+    <t>めんせつ</t>
+  </si>
+  <si>
+    <t>面接</t>
+  </si>
+  <si>
+    <t>phỏng vấn</t>
+  </si>
+  <si>
+    <t>cầm tay đứng trực tiếp nói chuyện với người con gái mình yêu</t>
+  </si>
+  <si>
+    <t>せっきん</t>
+  </si>
+  <si>
+    <t>接近</t>
+  </si>
+  <si>
+    <t>tiếp cận</t>
+  </si>
+  <si>
+    <t>せっする</t>
+  </si>
+  <si>
+    <t>接する</t>
+  </si>
+  <si>
+    <t>tiếp xúc</t>
+  </si>
+  <si>
+    <t>授</t>
+  </si>
+  <si>
+    <t>thụ</t>
+  </si>
+  <si>
+    <t>じゅぎょう</t>
+  </si>
+  <si>
+    <t>授業</t>
+  </si>
+  <si>
+    <t>giờ học</t>
+  </si>
+  <si>
+    <t>dùng Tay truyền thụ những gì đã nhận được(Thụ)</t>
+  </si>
+  <si>
+    <t>さずかった</t>
+  </si>
+  <si>
+    <t>授かった</t>
+  </si>
+  <si>
+    <t>được truyền thụ(trao)</t>
+  </si>
+  <si>
+    <t>さずけた</t>
+  </si>
+  <si>
+    <t>授けた</t>
+  </si>
+  <si>
+    <t>được trao(truyền thụ)</t>
+  </si>
+  <si>
+    <t>きょうじゅ</t>
+  </si>
+  <si>
+    <t>教授</t>
+  </si>
+  <si>
+    <t>giáo sư</t>
   </si>
   <si>
     <t>công thức</t>
@@ -4681,10 +4978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I271"/>
+  <dimension ref="A1:I297"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A801" workbookViewId="0">
-      <selection activeCell="A900" sqref="A2:XFD900"/>
+    <sheetView tabSelected="1" topLeftCell="A288" workbookViewId="0">
+      <selection activeCell="A298" sqref="A298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75"/>
@@ -8696,6 +8993,388 @@
       </c>
       <c r="E271" s="1" t="s">
         <v>1035</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7">
+      <c r="A272" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D272" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="E272" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="F272" s="1">
+        <v>5</v>
+      </c>
+      <c r="G272" s="1" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7">
+      <c r="C273" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="D273" s="1" t="s">
+        <v>1043</v>
+      </c>
+      <c r="E273" s="1" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7">
+      <c r="C274" s="1" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D274" s="1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E274" s="1" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="275" spans="1:7">
+      <c r="C275" s="1" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D275" s="1" t="s">
+        <v>1049</v>
+      </c>
+      <c r="E275" s="1" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="276" spans="1:7">
+      <c r="C276" s="1" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D276" s="1" t="s">
+        <v>1052</v>
+      </c>
+      <c r="E276" s="1" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="277" spans="1:7">
+      <c r="A277" s="1" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C277" s="1" t="s">
+        <v>1056</v>
+      </c>
+      <c r="D277" s="1" t="s">
+        <v>1057</v>
+      </c>
+      <c r="E277" s="1" t="s">
+        <v>1058</v>
+      </c>
+      <c r="F277" s="1">
+        <v>8</v>
+      </c>
+      <c r="G277" s="1" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="278" spans="1:7">
+      <c r="C278" s="1" t="s">
+        <v>1060</v>
+      </c>
+      <c r="D278" s="1" t="s">
+        <v>1061</v>
+      </c>
+      <c r="E278" s="1" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="279" spans="1:7">
+      <c r="C279" s="1" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D279" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E279" s="1" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="280" spans="1:7">
+      <c r="A280" s="1" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C280" s="1" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D280" s="1" t="s">
+        <v>1069</v>
+      </c>
+      <c r="E280" s="1" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F280" s="1">
+        <v>9</v>
+      </c>
+      <c r="G280" s="1" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="281" spans="1:7">
+      <c r="C281" s="1" t="s">
+        <v>1072</v>
+      </c>
+      <c r="D281" s="1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="E281" s="1" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="282" spans="1:7">
+      <c r="A282" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D282" s="1" t="s">
+        <v>1078</v>
+      </c>
+      <c r="E282" s="1" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F282" s="1">
+        <v>11</v>
+      </c>
+      <c r="G282" s="1" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="283" spans="1:7">
+      <c r="A283" s="1" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C283" s="1" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D283" s="1" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E283" s="1" t="s">
+        <v>1085</v>
+      </c>
+      <c r="F283" s="1">
+        <v>7</v>
+      </c>
+      <c r="G283" s="1" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="284" spans="1:7">
+      <c r="C284" s="1" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D284" s="1" t="s">
+        <v>1088</v>
+      </c>
+      <c r="E284" s="1" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="285" spans="1:7">
+      <c r="C285" s="1" t="s">
+        <v>1090</v>
+      </c>
+      <c r="D285" s="1" t="s">
+        <v>1091</v>
+      </c>
+      <c r="E285" s="1" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="286" spans="1:7">
+      <c r="C286" s="1" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D286" s="1" t="s">
+        <v>1094</v>
+      </c>
+      <c r="E286" s="1" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7">
+      <c r="A287" s="1" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>1097</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D287" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E287" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F287" s="1">
+        <v>8</v>
+      </c>
+      <c r="G287" s="1" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="288" spans="1:7">
+      <c r="C288" s="1" t="s">
+        <v>1099</v>
+      </c>
+      <c r="D288" s="1" t="s">
+        <v>1100</v>
+      </c>
+      <c r="E288" s="1" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="289" spans="1:7">
+      <c r="C289" s="1" t="s">
+        <v>1102</v>
+      </c>
+      <c r="D289" s="1" t="s">
+        <v>1103</v>
+      </c>
+      <c r="E289" s="1" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="290" spans="1:7">
+      <c r="C290" s="1" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D290" s="1" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E290" s="1" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7">
+      <c r="A291" s="1" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D291" s="1" t="s">
+        <v>1111</v>
+      </c>
+      <c r="E291" s="1" t="s">
+        <v>1112</v>
+      </c>
+      <c r="F291" s="1">
+        <v>11</v>
+      </c>
+      <c r="G291" s="1" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="292" spans="1:7">
+      <c r="C292" s="1" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D292" s="1" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E292" s="1" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="293" spans="1:7">
+      <c r="C293" s="1" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D293" s="1" t="s">
+        <v>1118</v>
+      </c>
+      <c r="E293" s="1" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7">
+      <c r="A294" s="1" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B294" s="1" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D294" s="1" t="s">
+        <v>1123</v>
+      </c>
+      <c r="E294" s="1" t="s">
+        <v>1124</v>
+      </c>
+      <c r="F294" s="1">
+        <v>11</v>
+      </c>
+      <c r="G294" s="1" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="295" spans="1:7">
+      <c r="C295" s="1" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D295" s="1" t="s">
+        <v>1127</v>
+      </c>
+      <c r="E295" s="1" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="296" spans="1:7">
+      <c r="C296" s="1" t="s">
+        <v>1129</v>
+      </c>
+      <c r="D296" s="1" t="s">
+        <v>1130</v>
+      </c>
+      <c r="E296" s="1" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="297" spans="1:7">
+      <c r="C297" s="1" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D297" s="1" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E297" s="1" t="s">
+        <v>1134</v>
       </c>
     </row>
   </sheetData>
@@ -8729,50 +9408,50 @@
   <sheetData>
     <row r="1" spans="1:22" ht="18.75">
       <c r="A1" s="2" t="s">
-        <v>1036</v>
+        <v>1135</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1037</v>
+        <v>1136</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1038</v>
+        <v>1137</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1039</v>
+        <v>1138</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1040</v>
+        <v>1139</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>1041</v>
+        <v>1140</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>1042</v>
+        <v>1141</v>
       </c>
       <c r="H1" s="2"/>
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:22" ht="18.75">
       <c r="A2" s="4" t="s">
-        <v>1043</v>
+        <v>1142</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1044</v>
+        <v>1143</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D2" s="1">
         <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>1047</v>
+        <v>1146</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1048</v>
+        <v>1147</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -8787,15 +9466,15 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>1049</v>
+        <v>1148</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>1050</v>
+        <v>1149</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -8810,15 +9489,15 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
-        <v>1051</v>
+        <v>1150</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>1052</v>
+        <v>1151</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -8831,25 +9510,25 @@
     </row>
     <row r="5" spans="1:22" ht="18.75">
       <c r="A5" s="3" t="s">
-        <v>1053</v>
+        <v>1152</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1054</v>
+        <v>1153</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D5" s="1">
         <v>46</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>1055</v>
+        <v>1154</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>1056</v>
+        <v>1155</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -8864,15 +9543,15 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>1057</v>
+        <v>1156</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>1058</v>
+        <v>1157</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -8887,15 +9566,15 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>1059</v>
+        <v>1158</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>1060</v>
+        <v>1159</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -8908,25 +9587,25 @@
     </row>
     <row r="8" spans="1:22" ht="18.75">
       <c r="A8" s="1" t="s">
-        <v>1061</v>
+        <v>1160</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1062</v>
+        <v>1161</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D8" s="1">
         <v>46</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>1047</v>
+        <v>1146</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>1063</v>
+        <v>1162</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -8941,13 +9620,13 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>1064</v>
+        <v>1163</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1065</v>
+        <v>1164</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -8960,25 +9639,25 @@
     </row>
     <row r="10" spans="1:22" ht="18.75">
       <c r="A10" s="1" t="s">
-        <v>1066</v>
+        <v>1165</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1067</v>
+        <v>1166</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D10" s="1">
         <v>45</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>1068</v>
+        <v>1167</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>1069</v>
+        <v>1168</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -9000,15 +9679,15 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>1070</v>
+        <v>1169</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>1071</v>
+        <v>1170</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -9028,25 +9707,25 @@
     </row>
     <row r="12" spans="1:22" ht="18.75">
       <c r="A12" s="1" t="s">
-        <v>1072</v>
+        <v>1171</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1073</v>
+        <v>1172</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D12" s="1">
         <v>45</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>1074</v>
+        <v>1173</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>1075</v>
+        <v>1174</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -9068,15 +9747,15 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>1076</v>
+        <v>1175</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>1077</v>
+        <v>1176</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -9096,25 +9775,25 @@
     </row>
     <row r="14" spans="1:22" ht="18.75">
       <c r="A14" s="6" t="s">
-        <v>1078</v>
+        <v>1177</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1079</v>
+        <v>1178</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D14" s="1">
         <v>44</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>1080</v>
+        <v>1179</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>1081</v>
+        <v>1180</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -9136,15 +9815,15 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>1082</v>
+        <v>1181</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>1083</v>
+        <v>1182</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -9164,25 +9843,25 @@
     </row>
     <row r="16" spans="1:22" ht="18.75">
       <c r="A16" s="1" t="s">
-        <v>1084</v>
+        <v>1183</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1085</v>
+        <v>1184</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D16" s="1">
         <v>44</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>1086</v>
+        <v>1185</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>1087</v>
+        <v>1186</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -9204,15 +9883,15 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>1088</v>
+        <v>1187</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>1089</v>
+        <v>1188</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -9232,25 +9911,25 @@
     </row>
     <row r="18" spans="1:22" ht="18.75">
       <c r="A18" s="1" t="s">
-        <v>1090</v>
+        <v>1189</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>1091</v>
+        <v>1190</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D18" s="1">
         <v>44</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>1092</v>
+        <v>1191</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>1093</v>
+        <v>1192</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -9272,15 +9951,15 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
-        <v>1094</v>
+        <v>1193</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>1095</v>
+        <v>1194</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -9300,25 +9979,25 @@
     </row>
     <row r="20" spans="1:22" ht="56.25">
       <c r="A20" s="3" t="s">
-        <v>1096</v>
+        <v>1195</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>1097</v>
+        <v>1196</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D20" s="1">
         <v>43</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>1098</v>
+        <v>1197</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>1099</v>
+        <v>1198</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -9340,15 +10019,15 @@
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>1100</v>
+        <v>1199</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>1101</v>
+        <v>1200</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -9370,15 +10049,15 @@
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>1102</v>
+        <v>1201</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>1103</v>
+        <v>1202</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -9400,15 +10079,15 @@
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>1104</v>
+        <v>1203</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>1105</v>
+        <v>1204</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -9428,25 +10107,25 @@
     </row>
     <row r="24" spans="1:22" ht="18.75">
       <c r="A24" s="1" t="s">
-        <v>1106</v>
+        <v>1205</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1107</v>
+        <v>1206</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D24" s="1">
         <v>43</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>1108</v>
+        <v>1207</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>1109</v>
+        <v>1208</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -9468,15 +10147,15 @@
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>1110</v>
+        <v>1209</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>1111</v>
+        <v>1210</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -9496,25 +10175,25 @@
     </row>
     <row r="26" spans="1:22" ht="18.75">
       <c r="A26" s="1" t="s">
-        <v>1112</v>
+        <v>1211</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>1113</v>
+        <v>1212</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D26" s="1">
         <v>42</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>1114</v>
+        <v>1213</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>1115</v>
+        <v>1214</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -9524,15 +10203,15 @@
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>1116</v>
+        <v>1215</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>1117</v>
+        <v>1216</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -9540,25 +10219,25 @@
     </row>
     <row r="28" spans="1:22" ht="18.75">
       <c r="A28" s="1" t="s">
-        <v>1118</v>
+        <v>1217</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>1119</v>
+        <v>1218</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D28" s="1">
         <v>42</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>1120</v>
+        <v>1219</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>1121</v>
+        <v>1220</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -9568,15 +10247,15 @@
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
-        <v>1122</v>
+        <v>1221</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>1123</v>
+        <v>1222</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -9586,15 +10265,15 @@
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1" t="s">
-        <v>1124</v>
+        <v>1223</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>1125</v>
+        <v>1224</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -9602,25 +10281,25 @@
     </row>
     <row r="31" spans="1:22" ht="18.75">
       <c r="A31" s="1" t="s">
-        <v>1126</v>
+        <v>1225</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>1127</v>
+        <v>1226</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D31" s="1">
         <v>42</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>1128</v>
+        <v>1227</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>1129</v>
+        <v>1228</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -9628,25 +10307,25 @@
     </row>
     <row r="32" spans="1:22" ht="18.75">
       <c r="A32" s="1" t="s">
-        <v>1130</v>
+        <v>1229</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1131</v>
+        <v>1230</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D32" s="1">
         <v>41</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>1132</v>
+        <v>1231</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>1133</v>
+        <v>1232</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -9656,15 +10335,15 @@
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
-        <v>1134</v>
+        <v>1233</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>1135</v>
+        <v>1234</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -9674,15 +10353,15 @@
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
-        <v>1136</v>
+        <v>1235</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>1137</v>
+        <v>1236</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -9690,25 +10369,25 @@
     </row>
     <row r="35" spans="1:10" ht="18.75">
       <c r="A35" s="1" t="s">
-        <v>1138</v>
+        <v>1237</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1139</v>
+        <v>1238</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D35" s="1">
         <v>41</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>1140</v>
+        <v>1239</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>1141</v>
+        <v>1240</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -9718,15 +10397,15 @@
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>1142</v>
+        <v>1241</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>1143</v>
+        <v>1242</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
@@ -9734,25 +10413,25 @@
     </row>
     <row r="37" spans="1:10" ht="18.75">
       <c r="A37" s="1" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>1144</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>1145</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>1045</v>
       </c>
       <c r="D37" s="1">
         <v>41</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>1146</v>
+        <v>1245</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>1147</v>
+        <v>1246</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
@@ -9762,15 +10441,15 @@
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1" t="s">
-        <v>1148</v>
+        <v>1247</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>1149</v>
+        <v>1248</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
@@ -9778,25 +10457,25 @@
     </row>
     <row r="39" spans="1:10" ht="18.75">
       <c r="A39" s="1" t="s">
-        <v>1150</v>
+        <v>1249</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>1151</v>
+        <v>1250</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D39" s="1">
         <v>41</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>1152</v>
+        <v>1251</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>1153</v>
+        <v>1252</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
@@ -9806,15 +10485,15 @@
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1" t="s">
-        <v>1154</v>
+        <v>1253</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>1155</v>
+        <v>1254</v>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
@@ -9822,801 +10501,801 @@
     </row>
     <row r="41" spans="1:10" ht="18.75">
       <c r="A41" s="1" t="s">
-        <v>1156</v>
+        <v>1255</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>1157</v>
+        <v>1256</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D41" s="1">
         <v>40</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>1158</v>
+        <v>1257</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>1159</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="18.75">
       <c r="C42" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>1160</v>
+        <v>1259</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>1161</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="18.75">
       <c r="C43" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>1162</v>
+        <v>1261</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>1163</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="18.75">
       <c r="A44" t="s">
-        <v>1164</v>
+        <v>1263</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>1165</v>
+        <v>1264</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D44" s="1">
         <v>40</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>1166</v>
+        <v>1265</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>1167</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="18.75">
       <c r="C45" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>1168</v>
+        <v>1267</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>1169</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="18.75">
       <c r="C46" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>1170</v>
+        <v>1269</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>1171</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="18.75">
       <c r="A47" t="s">
-        <v>1172</v>
+        <v>1271</v>
       </c>
       <c r="B47" t="s">
-        <v>1173</v>
+        <v>1272</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D47">
         <v>40</v>
       </c>
       <c r="E47" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>1174</v>
+        <v>1273</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>1175</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="18.75">
       <c r="C48" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>1176</v>
+        <v>1275</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>1177</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="18.75">
       <c r="C49" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>1178</v>
+        <v>1277</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>1179</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="18.75">
       <c r="A50" t="s">
-        <v>1180</v>
+        <v>1279</v>
       </c>
       <c r="B50" t="s">
-        <v>1181</v>
+        <v>1280</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D50">
         <v>40</v>
       </c>
       <c r="E50" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>1182</v>
+        <v>1281</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>1183</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="18.75">
       <c r="C51" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>1184</v>
+        <v>1283</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>1185</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="18.75">
       <c r="C52" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>1186</v>
+        <v>1285</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>1187</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="72.75">
       <c r="A53" t="s">
-        <v>1188</v>
+        <v>1287</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>1189</v>
+        <v>1288</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D53">
         <v>39</v>
       </c>
       <c r="E53" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>1190</v>
+        <v>1289</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>1191</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="18.75">
       <c r="C54" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>1192</v>
+        <v>1291</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>1193</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="18.75">
       <c r="C55" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>1194</v>
+        <v>1293</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>1195</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="18.75">
       <c r="C56" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>1196</v>
+        <v>1295</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>1197</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="18.75">
       <c r="C57" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>1198</v>
+        <v>1297</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>1199</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="18.75">
       <c r="A58" t="s">
-        <v>1200</v>
+        <v>1299</v>
       </c>
       <c r="B58" t="s">
-        <v>1201</v>
+        <v>1300</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D58">
         <v>39</v>
       </c>
       <c r="E58" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>1202</v>
+        <v>1301</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>1203</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="18.75">
       <c r="C59" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>1204</v>
+        <v>1303</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>1205</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="18.75">
       <c r="A60" t="s">
-        <v>1206</v>
+        <v>1305</v>
       </c>
       <c r="B60" t="s">
-        <v>1207</v>
+        <v>1306</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D60">
         <v>39</v>
       </c>
       <c r="E60" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>1208</v>
+        <v>1307</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>1209</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="18.75">
       <c r="C61" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>1210</v>
+        <v>1309</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>1211</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="58.5">
       <c r="A62" t="s">
-        <v>1212</v>
+        <v>1311</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>1213</v>
+        <v>1312</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D62">
         <v>38</v>
       </c>
       <c r="E62" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>1214</v>
+        <v>1313</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>1215</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="18.75">
       <c r="C63" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>1216</v>
+        <v>1315</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>1217</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="18.75">
       <c r="C64" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>1218</v>
+        <v>1317</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>1219</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="18.75">
       <c r="C65" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>1220</v>
+        <v>1319</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>1221</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="18.75">
       <c r="C66" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>1222</v>
+        <v>1321</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>1223</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="18.75">
       <c r="A67" t="s">
-        <v>1224</v>
+        <v>1323</v>
       </c>
       <c r="B67" t="s">
-        <v>1225</v>
+        <v>1324</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D67">
         <v>47</v>
       </c>
       <c r="E67" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>1226</v>
+        <v>1325</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>1227</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="18.75">
       <c r="C68" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>1228</v>
+        <v>1327</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>1229</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="18.75">
       <c r="C69" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>1230</v>
+        <v>1329</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>1231</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="18.75">
       <c r="A70" t="s">
-        <v>1232</v>
+        <v>1331</v>
       </c>
       <c r="B70" t="s">
-        <v>1233</v>
+        <v>1332</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D70">
         <v>47</v>
       </c>
       <c r="E70" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>1234</v>
+        <v>1333</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>1235</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="18.75">
       <c r="F71" s="1" t="s">
-        <v>1236</v>
+        <v>1335</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>1237</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="18.75">
       <c r="F72" s="1" t="s">
-        <v>1238</v>
+        <v>1337</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>1239</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="18.75">
       <c r="A73" t="s">
-        <v>1240</v>
+        <v>1339</v>
       </c>
       <c r="B73" t="s">
-        <v>1241</v>
+        <v>1340</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D73">
         <v>26</v>
       </c>
       <c r="E73" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>1242</v>
+        <v>1341</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>1243</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="18.75">
       <c r="F74" s="1" t="s">
-        <v>1244</v>
+        <v>1343</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>1245</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="18.75">
       <c r="F75" s="1" t="s">
-        <v>1246</v>
+        <v>1345</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>1247</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="18.75">
       <c r="A76" t="s">
-        <v>1248</v>
+        <v>1347</v>
       </c>
       <c r="B76" t="s">
-        <v>1249</v>
+        <v>1348</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D76">
         <v>27</v>
       </c>
       <c r="E76" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>1250</v>
+        <v>1349</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>1251</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="18.75">
       <c r="F77" s="1" t="s">
-        <v>1252</v>
+        <v>1351</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>1253</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="18.75">
       <c r="A78" t="s">
-        <v>1254</v>
+        <v>1353</v>
       </c>
       <c r="B78" t="s">
-        <v>1255</v>
+        <v>1354</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D78">
         <v>27</v>
       </c>
       <c r="E78" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>1256</v>
+        <v>1355</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>1257</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="18.75">
       <c r="F79" s="1" t="s">
-        <v>1258</v>
+        <v>1357</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>1259</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="18.75">
       <c r="A80" t="s">
-        <v>1260</v>
+        <v>1359</v>
       </c>
       <c r="B80" t="s">
-        <v>1261</v>
+        <v>1360</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D80">
         <v>27</v>
       </c>
       <c r="E80" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>1262</v>
+        <v>1361</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>1263</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="18.75">
       <c r="F81" s="1" t="s">
-        <v>1264</v>
+        <v>1363</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>1265</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="18.75">
       <c r="A82" t="s">
-        <v>1266</v>
+        <v>1365</v>
       </c>
       <c r="B82" t="s">
-        <v>1267</v>
+        <v>1366</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D82">
         <v>28</v>
       </c>
       <c r="E82" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>1268</v>
+        <v>1367</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>1269</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="18.75">
       <c r="F83" s="1" t="s">
-        <v>1270</v>
+        <v>1369</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>1271</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="18.75">
       <c r="A84" t="s">
-        <v>1272</v>
+        <v>1371</v>
       </c>
       <c r="B84" t="s">
-        <v>1273</v>
+        <v>1372</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D84">
         <v>28</v>
       </c>
       <c r="E84" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>1274</v>
+        <v>1373</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>1275</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="18.75">
       <c r="F85" s="1" t="s">
-        <v>1276</v>
+        <v>1375</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>1277</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="18.75">
       <c r="A86" t="s">
-        <v>1278</v>
+        <v>1377</v>
       </c>
       <c r="B86" t="s">
-        <v>1279</v>
+        <v>1378</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D86">
         <v>28</v>
       </c>
       <c r="E86" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>1280</v>
+        <v>1379</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>1281</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="18.75">
       <c r="A87" t="s">
-        <v>1282</v>
+        <v>1381</v>
       </c>
       <c r="B87" t="s">
-        <v>1283</v>
+        <v>1382</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D87">
         <v>29</v>
       </c>
       <c r="E87" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>1284</v>
+        <v>1383</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>1285</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="18.75">
       <c r="F88" s="1" t="s">
-        <v>1286</v>
+        <v>1385</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>1287</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="18.75">
       <c r="F89" s="1" t="s">
-        <v>1288</v>
+        <v>1387</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>1289</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="18.75">
       <c r="A90" t="s">
-        <v>1290</v>
+        <v>1389</v>
       </c>
       <c r="B90" t="s">
-        <v>1291</v>
+        <v>1390</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D90">
         <v>29</v>
       </c>
       <c r="E90" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>1292</v>
+        <v>1391</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>1293</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="18.75">
       <c r="F91" s="1" t="s">
-        <v>1294</v>
+        <v>1393</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>1295</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="18.75">
       <c r="F92" s="1" t="s">
-        <v>1296</v>
+        <v>1395</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>1297</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="18.75">
       <c r="F93" s="1" t="s">
-        <v>1298</v>
+        <v>1397</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>1299</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="18.75">
       <c r="A94" t="s">
-        <v>1300</v>
+        <v>1399</v>
       </c>
       <c r="B94" t="s">
-        <v>1301</v>
+        <v>1400</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1045</v>
+        <v>1144</v>
       </c>
       <c r="D94">
         <v>30</v>
       </c>
       <c r="E94" t="s">
-        <v>1046</v>
+        <v>1145</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>1302</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="18.75">
       <c r="F95" s="1" t="s">
-        <v>1303</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="18.75">
       <c r="F96" s="1" t="s">
-        <v>1304</v>
+        <v>1403</v>
       </c>
     </row>
   </sheetData>

</xml_diff>